<commit_message>
vault backup: 2024-09-30 17:43:26
</commit_message>
<xml_diff>
--- a/2024-2/Evaluación de proyectos/Excels/Ejercicios_sol_1.xlsx
+++ b/2024-2/Evaluación de proyectos/Excels/Ejercicios_sol_1.xlsx
@@ -2,27 +2,28 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivaaan\Desktop\git\Apuntes_2024\2024-2\Evaluación de proyectos\Excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IVAN\Desktop\Codes\Apuntes_2024\2024-2\Evaluación de proyectos\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{711AB42A-8C0D-423C-9382-B5AA196DDA1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF3F871-6C4B-4D31-8E1E-08EA24E03523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{C81B0A03-BDB8-4836-9CA0-B318B652DAA5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{C81B0A03-BDB8-4836-9CA0-B318B652DAA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Ej Aprovación de credito" sheetId="1" r:id="rId1"/>
     <sheet name="Tabla dinámica" sheetId="2" r:id="rId2"/>
     <sheet name="Flujo de caja" sheetId="3" r:id="rId3"/>
+    <sheet name="FORMULARIO" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Tabla dinámica'!$B$3:$E$24</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="4" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="89">
   <si>
     <t>TASA REAL EFECTIVA CREDITO</t>
   </si>
@@ -134,18 +135,197 @@
   </si>
   <si>
     <t>Total general</t>
+  </si>
+  <si>
+    <t>INGRESOS</t>
+  </si>
+  <si>
+    <t>CANTIDAD</t>
+  </si>
+  <si>
+    <t>PRECIO</t>
+  </si>
+  <si>
+    <t>COSTOS</t>
+  </si>
+  <si>
+    <t>FIJOS</t>
+  </si>
+  <si>
+    <t>VARIABLE</t>
+  </si>
+  <si>
+    <t>DEPRECIACIÓN</t>
+  </si>
+  <si>
+    <t>INTERESES</t>
+  </si>
+  <si>
+    <t>MANTENCIÓN</t>
+  </si>
+  <si>
+    <t>AMORTIZACIÓN</t>
+  </si>
+  <si>
+    <t>&lt;- COMPUESTO</t>
+  </si>
+  <si>
+    <t>FORMA 2</t>
+  </si>
+  <si>
+    <t>FORMA 1</t>
+  </si>
+  <si>
+    <t>INTERES COMPUESTO</t>
+  </si>
+  <si>
+    <t>&lt;- SIMPLE</t>
+  </si>
+  <si>
+    <t>INTERES SIMPLE</t>
+  </si>
+  <si>
+    <t>NUM MESES</t>
+  </si>
+  <si>
+    <t>TASA INTERES MENSUAL</t>
+  </si>
+  <si>
+    <t>SALDO INSOLUTO</t>
+  </si>
+  <si>
+    <t>DATOS</t>
+  </si>
+  <si>
+    <t>MULTAS</t>
+  </si>
+  <si>
+    <t>TASA INTERES EFECTIVA</t>
+  </si>
+  <si>
+    <t>VALOR PRESENTE DE CUOTAS PAGADAS</t>
+  </si>
+  <si>
+    <t>CREDITO</t>
+  </si>
+  <si>
+    <t>MONTO CUOTA A PAGAR</t>
+  </si>
+  <si>
+    <t>MENSUALES</t>
+  </si>
+  <si>
+    <t>MENSUAL</t>
+  </si>
+  <si>
+    <t>TRIMESTRALES</t>
+  </si>
+  <si>
+    <t>SEMESTRALES</t>
+  </si>
+  <si>
+    <t>ANUALES</t>
+  </si>
+  <si>
+    <t>TRIMESTRAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>SEMESTRAL</t>
+  </si>
+  <si>
+    <t>ANUAL</t>
+  </si>
+  <si>
+    <t>CUOTAS</t>
+  </si>
+  <si>
+    <t>COMPOSICION</t>
+  </si>
+  <si>
+    <t>INT. ANUAL NOMINAL</t>
+  </si>
+  <si>
+    <t>CAPITAL INICIAL / VP</t>
+  </si>
+  <si>
+    <t>CAPITAL FINAL / VF</t>
+  </si>
+  <si>
+    <t>VP = CAP.INICIAL</t>
+  </si>
+  <si>
+    <t>CAP. FINAL</t>
+  </si>
+  <si>
+    <t>PERIODOS</t>
+  </si>
+  <si>
+    <t>CAP. INICIAL</t>
+  </si>
+  <si>
+    <t>VF = CAP.FINAL</t>
+  </si>
+  <si>
+    <t>INTERÉS COMPUESTO</t>
+  </si>
+  <si>
+    <t>FORMULARIO</t>
+  </si>
+  <si>
+    <t>MONTO</t>
+  </si>
+  <si>
+    <t>UTILIDAD</t>
+  </si>
+  <si>
+    <t>IMPUESTO</t>
+  </si>
+  <si>
+    <t>UTILIDAD DESPUES IMPUESTO</t>
+  </si>
+  <si>
+    <t>INVERSIONES</t>
+  </si>
+  <si>
+    <t>TERRENO</t>
+  </si>
+  <si>
+    <t>EDIFICACION</t>
+  </si>
+  <si>
+    <t>MAQUINARIA</t>
+  </si>
+  <si>
+    <t>CAPITAL TRABAJO</t>
+  </si>
+  <si>
+    <t>FLUJO</t>
+  </si>
+  <si>
+    <t>VAN</t>
+  </si>
+  <si>
+    <t>CAPM</t>
+  </si>
+  <si>
+    <t>TIR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="5">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]&quot;$&quot;\-#,##0"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;\-#,##0.00"/>
     <numFmt numFmtId="42" formatCode="_ &quot;$&quot;* #,##0_ ;_ &quot;$&quot;* \-#,##0_ ;_ &quot;$&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;$&quot;* #,##0.00_ ;_ &quot;$&quot;* \-#,##0.00_ ;_ &quot;$&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="168" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,16 +355,64 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="36"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -233,12 +461,310 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -274,10 +800,208 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Moneda [0]" xfId="1" builtinId="7"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentaje" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -338,17 +1062,7 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="5.71402522453456E-2"/>
-          <c:y val="0.17525630898079489"/>
-          <c:w val="0.9208854407904894"/>
-          <c:h val="0.74061488673139153"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -371,22 +1085,16 @@
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent2"/>
+                  <a:schemeClr val="accent1"/>
                 </a:solidFill>
                 <a:prstDash val="sysDot"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="exp"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-3.0969398348533007E-2"/>
-                  <c:y val="-5.0686723861009912E-2"/>
-                </c:manualLayout>
-              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -421,69 +1129,36 @@
             <c:strRef>
               <c:f>'Tabla dinámica'!$C$4:$C$24</c:f>
               <c:strCache>
-                <c:ptCount val="21"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>PRODUCTO A</c:v>
+                  <c:v>PRODUCTO B</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>PRODUCTO B</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>PRODUCTO A</c:v>
+                  <c:v>PRODUCTO B</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>PRODUCTO B</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>PRODUCTO A</c:v>
+                  <c:v>PRODUCTO B</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>PRODUCTO B</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>PRODUCTO A</c:v>
+                  <c:v>PRODUCTO B</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>PRODUCTO B</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>PRODUCTO A</c:v>
+                  <c:v>PRODUCTO B</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>PRODUCTO B</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>PRODUCTO A</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>PRODUCTO B</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>PRODUCTO A</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>PRODUCTO B</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>PRODUCTO A</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>PRODUCTO B</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>PRODUCTO A</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>PRODUCTO B</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>PRODUCTO A</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>PRODUCTO B</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>PRODUCTO A</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -493,69 +1168,36 @@
               <c:f>'Tabla dinámica'!$D$4:$D$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>95</c:v>
+                  <c:v>152</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>117</c:v>
+                  <c:v>220</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>152</c:v>
+                  <c:v>350</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>120</c:v>
+                  <c:v>570</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>220</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>139</c:v>
+                  <c:v>1300</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>350</c:v>
+                  <c:v>1900</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>158</c:v>
+                  <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>570</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>165</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>800</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>171</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1300</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>175</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1900</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>180</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>3000</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>186</c:v>
-                </c:pt>
-                <c:pt idx="19">
                   <c:v>4400</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>198</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -563,7 +1205,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-985D-4DD3-89F3-866A3DA93470}"/>
+              <c16:uniqueId val="{00000000-389C-461A-9067-2C08F0287A51}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -576,11 +1218,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="891591151"/>
-        <c:axId val="823594127"/>
+        <c:axId val="1471512320"/>
+        <c:axId val="1471508480"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="891591151"/>
+        <c:axId val="1471512320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -623,7 +1265,7 @@
             <a:endParaRPr lang="es-CL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="823594127"/>
+        <c:crossAx val="1471508480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -631,7 +1273,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="823594127"/>
+        <c:axId val="1471508480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -682,7 +1324,7 @@
             <a:endParaRPr lang="es-CL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="891591151"/>
+        <c:crossAx val="1471512320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1347,23 +1989,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Gráfico 2">
+        <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A370F975-0DFD-C25F-371E-7D7A5751D901}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A49DBE1B-FA44-3349-72AF-C2B4E132C8B1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1389,22 +2031,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>55833</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>448587</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>48908</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
+        <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C03B8867-BD91-41FC-B364-93B1529FEAD1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB8E5186-3952-F092-3737-FFA48A54CA5E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1420,8 +2062,52 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="5478780" cy="4262073"/>
+          <a:off x="9525" y="0"/>
+          <a:ext cx="6535062" cy="9192908"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>534325</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>19455</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{056E0325-34B4-65C9-887B-2B3B7EAD005F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="9115425"/>
+          <a:ext cx="6630325" cy="2905530"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1433,15 +2119,290 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>118110</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>26670</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1224915" cy="775159"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AA294AE-93AB-4B62-91E2-252777C895AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3928110" y="1741170"/>
+          <a:ext cx="1224915" cy="775159"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>36195</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>59055</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1552797" cy="453451"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BEE2A19-FFD4-4112-A435-9C762C59C10D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2322195" y="1773555"/>
+          <a:ext cx="1552797" cy="453451"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4677428" cy="600159"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFEFD351-D836-459A-BAB9-42F1ADFCC450}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="6105525"/>
+          <a:ext cx="4677428" cy="600159"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1571844" cy="590632"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB884412-0BE0-4D0A-A66A-AB00A4065BF9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5362575" y="7153275"/>
+          <a:ext cx="1571844" cy="590632"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>188595</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1448002" cy="628738"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B2FE3FC-9021-4748-B7E2-D5093E7069D2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5440680" y="7999095"/>
+          <a:ext cx="1448002" cy="628738"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4371975" cy="887849"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagen 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECD086AC-7123-4C84-BC20-1180A1408940}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6267450" y="9134475"/>
+          <a:ext cx="4371975" cy="887849"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="6325483" cy="685896"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagen 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6600920-850F-4A15-8216-9B8EA830E959}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4314825" y="10020300"/>
+          <a:ext cx="6325483" cy="685896"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Ivaaan" refreshedDate="45558.719225462963" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="21" xr:uid="{659651B2-81AD-4185-B6CF-62E340A4EF58}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="IVAN" refreshedDate="45565.735745949074" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="21" xr:uid="{B98FC9E6-6D5E-4265-9919-719B74BFB05D}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="B3:D24" sheet="Tabla dinámica"/>
+    <worksheetSource ref="C3:D24" sheet="Tabla dinámica"/>
   </cacheSource>
-  <cacheFields count="3">
-    <cacheField name="AÑO" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2000" maxValue="2010"/>
-    </cacheField>
+  <cacheFields count="2">
     <cacheField name="PRODUCTO A" numFmtId="0">
       <sharedItems count="2">
         <s v="PRODUCTO A"/>
@@ -1463,107 +2424,86 @@
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="21">
   <r>
-    <n v="2000"/>
     <x v="0"/>
     <n v="100"/>
   </r>
   <r>
-    <n v="2000"/>
     <x v="1"/>
     <n v="95"/>
   </r>
   <r>
-    <n v="2001"/>
     <x v="0"/>
     <n v="117"/>
   </r>
   <r>
-    <n v="2001"/>
     <x v="1"/>
     <n v="152"/>
   </r>
   <r>
-    <n v="2002"/>
     <x v="0"/>
     <n v="120"/>
   </r>
   <r>
-    <n v="2002"/>
     <x v="1"/>
     <n v="220"/>
   </r>
   <r>
-    <n v="2003"/>
     <x v="0"/>
     <n v="139"/>
   </r>
   <r>
-    <n v="2003"/>
     <x v="1"/>
     <n v="350"/>
   </r>
   <r>
-    <n v="2004"/>
     <x v="0"/>
     <n v="158"/>
   </r>
   <r>
-    <n v="2004"/>
     <x v="1"/>
     <n v="570"/>
   </r>
   <r>
-    <n v="2005"/>
     <x v="0"/>
     <n v="165"/>
   </r>
   <r>
-    <n v="2005"/>
     <x v="1"/>
     <n v="800"/>
   </r>
   <r>
-    <n v="2006"/>
     <x v="0"/>
     <n v="171"/>
   </r>
   <r>
-    <n v="2006"/>
     <x v="1"/>
     <n v="1300"/>
   </r>
   <r>
-    <n v="2007"/>
     <x v="0"/>
     <n v="175"/>
   </r>
   <r>
-    <n v="2007"/>
     <x v="1"/>
     <n v="1900"/>
   </r>
   <r>
-    <n v="2008"/>
     <x v="0"/>
     <n v="180"/>
   </r>
   <r>
-    <n v="2008"/>
     <x v="1"/>
     <n v="3000"/>
   </r>
   <r>
-    <n v="2009"/>
     <x v="0"/>
     <n v="186"/>
   </r>
   <r>
-    <n v="2009"/>
     <x v="1"/>
     <n v="4400"/>
   </r>
   <r>
-    <n v="2010"/>
     <x v="0"/>
     <n v="198"/>
   </r>
@@ -1571,10 +2511,9 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5DFCB6D2-E0C9-44BF-B73B-270A51328F04}" name="TablaDinámica10" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="G3:H6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="3">
-    <pivotField showAll="0"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C56BEC62-8017-431D-B3BC-C82E605B6596}" name="TablaDinámica1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="H4:I7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
       <items count="3">
         <item x="0"/>
@@ -1585,7 +2524,7 @@
     <pivotField dataField="1" showAll="0"/>
   </pivotFields>
   <rowFields count="1">
-    <field x="1"/>
+    <field x="0"/>
   </rowFields>
   <rowItems count="3">
     <i>
@@ -1602,7 +2541,7 @@
     <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="Suma de VENTA UNIDS " fld="2" baseField="0" baseItem="0"/>
+    <dataField name="Suma de VENTA UNIDS " fld="1" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -1935,20 +2874,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16A51246-93CB-4F0A-B41E-2FA7CB8E0C7A}">
   <dimension ref="F2:K44"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="I46" sqref="I46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="6:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="6:11" x14ac:dyDescent="0.25">
       <c r="G2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1956,7 +2895,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="3" spans="6:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="6:11" x14ac:dyDescent="0.25">
       <c r="G3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1964,7 +2903,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="6:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="6:11" x14ac:dyDescent="0.25">
       <c r="G4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1973,7 +2912,7 @@
         <v>0.12682503013196977</v>
       </c>
     </row>
-    <row r="5" spans="6:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="6:11" x14ac:dyDescent="0.25">
       <c r="G5" s="2" t="s">
         <v>4</v>
       </c>
@@ -1987,7 +2926,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="6:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="6:11" x14ac:dyDescent="0.25">
       <c r="G6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1996,10 +2935,10 @@
         <v>2107535.6902545234</v>
       </c>
     </row>
-    <row r="7" spans="6:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="6:11" x14ac:dyDescent="0.25">
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="6:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="6:11" x14ac:dyDescent="0.25">
       <c r="G8" s="2" t="s">
         <v>10</v>
       </c>
@@ -2009,7 +2948,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="6:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="6:11" x14ac:dyDescent="0.25">
       <c r="G9" s="2" t="s">
         <v>6</v>
       </c>
@@ -2024,7 +2963,7 @@
         <v>8500000</v>
       </c>
     </row>
-    <row r="10" spans="6:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F10">
         <v>1</v>
       </c>
@@ -2045,7 +2984,7 @@
         <v>7470477.0658672191</v>
       </c>
     </row>
-    <row r="11" spans="6:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F11">
         <v>2</v>
       </c>
@@ -2066,7 +3005,7 @@
         <v>6310384.8545914944</v>
       </c>
     </row>
-    <row r="12" spans="6:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F12">
         <v>3</v>
       </c>
@@ -2087,7 +3026,7 @@
         <v>5003163.9136648625</v>
       </c>
     </row>
-    <row r="13" spans="6:11" ht="21" x14ac:dyDescent="0.4">
+    <row r="13" spans="6:11" ht="21" x14ac:dyDescent="0.35">
       <c r="F13">
         <v>4</v>
       </c>
@@ -2112,7 +3051,7 @@
         <v>3883170.1012676763</v>
       </c>
     </row>
-    <row r="14" spans="6:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F14">
         <v>5</v>
       </c>
@@ -2133,7 +3072,7 @@
         <v>1870330.9155350341</v>
       </c>
     </row>
-    <row r="15" spans="6:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F15">
         <v>6</v>
       </c>
@@ -2154,7 +3093,7 @@
         <v>-3.9581209421157837E-9</v>
       </c>
     </row>
-    <row r="18" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G18" s="15" t="s">
         <v>11</v>
       </c>
@@ -2162,7 +3101,7 @@
       <c r="I18" s="15"/>
       <c r="J18" s="15"/>
     </row>
-    <row r="19" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G19" s="2" t="s">
         <v>12</v>
       </c>
@@ -2172,7 +3111,7 @@
       </c>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G20" s="6">
         <f>-FV(8%,3,,3650000)</f>
         <v>4597948.8000000007</v>
@@ -2184,20 +3123,20 @@
       </c>
       <c r="J20" s="2"/>
     </row>
-    <row r="22" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G22" s="16" t="s">
         <v>14</v>
       </c>
       <c r="H22" s="17"/>
     </row>
-    <row r="23" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G23" s="18">
         <f>K13-I20</f>
         <v>1584195.701267676</v>
       </c>
       <c r="H23" s="19"/>
     </row>
-    <row r="24" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G24" s="2" t="s">
         <v>15</v>
       </c>
@@ -2205,7 +3144,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="25" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G25" s="2" t="s">
         <v>16</v>
       </c>
@@ -2213,7 +3152,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G26" s="2" t="s">
         <v>3</v>
       </c>
@@ -2222,7 +3161,7 @@
         <v>614721.02489998355</v>
       </c>
     </row>
-    <row r="27" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G27" s="2" t="s">
         <v>17</v>
       </c>
@@ -2232,7 +3171,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G28" s="2" t="s">
         <v>6</v>
       </c>
@@ -2247,7 +3186,7 @@
         <v>1584195.701267676</v>
       </c>
     </row>
-    <row r="29" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G29" s="9">
         <f>$H$24*J28</f>
         <v>126735.65610141408</v>
@@ -2265,7 +3204,7 @@
         <v>1096210.3324691064</v>
       </c>
     </row>
-    <row r="30" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G30" s="9">
         <f>$H$24*J29</f>
         <v>87696.826597528518</v>
@@ -2283,7 +3222,7 @@
         <v>569186.13416665141</v>
       </c>
     </row>
-    <row r="31" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G31" s="9">
         <f>$H$24*J30</f>
         <v>45534.890733332111</v>
@@ -2301,12 +3240,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="7:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G33" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="7:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="7:9" x14ac:dyDescent="0.25">
       <c r="H34" t="s">
         <v>20</v>
       </c>
@@ -2314,7 +3253,7 @@
         <v>1.03</v>
       </c>
     </row>
-    <row r="35" spans="7:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G35" s="2" t="s">
         <v>19</v>
       </c>
@@ -2325,7 +3264,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="7:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G36" s="2">
         <v>1</v>
       </c>
@@ -2337,7 +3276,7 @@
         <v>2046151.1555869158</v>
       </c>
     </row>
-    <row r="37" spans="7:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G37" s="2">
         <v>2</v>
       </c>
@@ -2349,7 +3288,7 @@
         <v>1986554.519987297</v>
       </c>
     </row>
-    <row r="38" spans="7:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G38" s="2">
         <v>3</v>
       </c>
@@ -2361,7 +3300,7 @@
         <v>1928693.7087255311</v>
       </c>
     </row>
-    <row r="39" spans="7:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G39" s="2">
         <v>4</v>
       </c>
@@ -2373,7 +3312,7 @@
         <v>1872518.1638111954</v>
       </c>
     </row>
-    <row r="40" spans="7:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G40" s="2">
         <v>5</v>
       </c>
@@ -2385,7 +3324,7 @@
         <v>530263.75602436229</v>
       </c>
     </row>
-    <row r="41" spans="7:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G41" s="2">
         <v>6</v>
       </c>
@@ -2397,7 +3336,7 @@
         <v>514819.18060617696</v>
       </c>
     </row>
-    <row r="42" spans="7:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G42" s="2">
         <v>7</v>
       </c>
@@ -2409,7 +3348,7 @@
         <v>499824.44719046302</v>
       </c>
     </row>
-    <row r="44" spans="7:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G44" s="20" t="s">
         <v>22</v>
       </c>
@@ -2433,23 +3372,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5C1D520-EAF6-40A7-AC3A-61C23BF36621}">
-  <dimension ref="B3:H24"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="B3:I24"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
         <v>23</v>
       </c>
@@ -2460,14 +3400,8 @@
         <v>25</v>
       </c>
       <c r="E3" s="12"/>
-      <c r="G3" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="2:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B4" s="12">
         <v>2000</v>
       </c>
@@ -2478,14 +3412,14 @@
         <v>100</v>
       </c>
       <c r="E4" s="12"/>
-      <c r="G4" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4">
-        <v>1709</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H4" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="12">
         <v>2000</v>
       </c>
@@ -2496,14 +3430,14 @@
         <v>95</v>
       </c>
       <c r="E5" s="12"/>
-      <c r="G5" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5">
-        <v>12787</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H5" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="103">
+        <v>1709</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B6" s="12">
         <v>2001</v>
       </c>
@@ -2514,14 +3448,14 @@
         <v>117</v>
       </c>
       <c r="E6" s="12"/>
-      <c r="G6" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6">
-        <v>14496</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H6" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="103">
+        <v>12787</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="12">
         <v>2001</v>
       </c>
@@ -2532,8 +3466,14 @@
         <v>152</v>
       </c>
       <c r="E7" s="12"/>
-    </row>
-    <row r="8" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H7" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="103">
+        <v>14496</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B8" s="12">
         <v>2002</v>
       </c>
@@ -2545,7 +3485,7 @@
       </c>
       <c r="E8" s="12"/>
     </row>
-    <row r="9" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="12">
         <v>2002</v>
       </c>
@@ -2557,7 +3497,7 @@
       </c>
       <c r="E9" s="12"/>
     </row>
-    <row r="10" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B10" s="12">
         <v>2003</v>
       </c>
@@ -2569,7 +3509,7 @@
       </c>
       <c r="E10" s="12"/>
     </row>
-    <row r="11" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="12">
         <v>2003</v>
       </c>
@@ -2581,7 +3521,7 @@
       </c>
       <c r="E11" s="12"/>
     </row>
-    <row r="12" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B12" s="12">
         <v>2004</v>
       </c>
@@ -2593,7 +3533,7 @@
       </c>
       <c r="E12" s="12"/>
     </row>
-    <row r="13" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="12">
         <v>2004</v>
       </c>
@@ -2605,7 +3545,7 @@
       </c>
       <c r="E13" s="12"/>
     </row>
-    <row r="14" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B14" s="12">
         <v>2005</v>
       </c>
@@ -2617,7 +3557,7 @@
       </c>
       <c r="E14" s="12"/>
     </row>
-    <row r="15" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="12">
         <v>2005</v>
       </c>
@@ -2629,7 +3569,7 @@
       </c>
       <c r="E15" s="12"/>
     </row>
-    <row r="16" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B16" s="12">
         <v>2006</v>
       </c>
@@ -2641,7 +3581,7 @@
       </c>
       <c r="E16" s="12"/>
     </row>
-    <row r="17" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="12">
         <v>2006</v>
       </c>
@@ -2653,7 +3593,7 @@
       </c>
       <c r="E17" s="12"/>
     </row>
-    <row r="18" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B18" s="12">
         <v>2007</v>
       </c>
@@ -2665,7 +3605,7 @@
       </c>
       <c r="E18" s="12"/>
     </row>
-    <row r="19" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="12">
         <v>2007</v>
       </c>
@@ -2677,7 +3617,7 @@
       </c>
       <c r="E19" s="12"/>
     </row>
-    <row r="20" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B20" s="12">
         <v>2008</v>
       </c>
@@ -2689,7 +3629,7 @@
       </c>
       <c r="E20" s="12"/>
     </row>
-    <row r="21" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="12">
         <v>2008</v>
       </c>
@@ -2701,7 +3641,7 @@
       </c>
       <c r="E21" s="12"/>
     </row>
-    <row r="22" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B22" s="12">
         <v>2009</v>
       </c>
@@ -2713,7 +3653,7 @@
       </c>
       <c r="E22" s="12"/>
     </row>
-    <row r="23" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="12">
         <v>2009</v>
       </c>
@@ -2725,7 +3665,7 @@
       </c>
       <c r="E23" s="12"/>
     </row>
-    <row r="24" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B24" s="12">
         <v>2010</v>
       </c>
@@ -2738,7 +3678,13 @@
       <c r="E24" s="12"/>
     </row>
   </sheetData>
-  <autoFilter ref="B3:E24" xr:uid="{D5C1D520-EAF6-40A7-AC3A-61C23BF36621}"/>
+  <autoFilter ref="B3:E24" xr:uid="{D5C1D520-EAF6-40A7-AC3A-61C23BF36621}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="PRODUCTO B"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
 </worksheet>
@@ -2746,12 +3692,1514 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C8269A2-8272-4B58-BB60-2DE0A7F360FB}">
-  <dimension ref="A1"/>
+  <dimension ref="J3:Q41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="10" width="11.42578125" style="21"/>
+    <col min="11" max="11" width="27" style="21" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" style="21"/>
+    <col min="13" max="13" width="14.5703125" style="21" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="11.42578125" style="21"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="M3" s="21">
+        <v>1</v>
+      </c>
+      <c r="N3" s="21">
+        <v>2</v>
+      </c>
+      <c r="O3" s="21">
+        <v>3</v>
+      </c>
+      <c r="P3" s="21">
+        <v>4</v>
+      </c>
+      <c r="Q3" s="21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="K4" s="22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="K5" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" s="21">
+        <v>1500</v>
+      </c>
+      <c r="N5" s="21">
+        <f>M5*(1+8%)</f>
+        <v>1620</v>
+      </c>
+      <c r="O5" s="21">
+        <f>N5*(1+8%)</f>
+        <v>1749.6000000000001</v>
+      </c>
+      <c r="P5" s="21">
+        <f>O5*(1+12%)</f>
+        <v>1959.5520000000004</v>
+      </c>
+      <c r="Q5" s="21">
+        <f>P5*(1+12%)</f>
+        <v>2194.6982400000006</v>
+      </c>
+    </row>
+    <row r="6" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="K6" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="M6" s="21">
+        <v>8000</v>
+      </c>
+      <c r="N6" s="21">
+        <f>M6*(1+2.5%)</f>
+        <v>8200</v>
+      </c>
+      <c r="O6" s="21">
+        <f t="shared" ref="O6:Q6" si="0">N6*(1+2.5%)</f>
+        <v>8405</v>
+      </c>
+      <c r="P6" s="21">
+        <f t="shared" si="0"/>
+        <v>8615.125</v>
+      </c>
+      <c r="Q6" s="21">
+        <f t="shared" si="0"/>
+        <v>8830.5031249999993</v>
+      </c>
+    </row>
+    <row r="7" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="K7" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="M7" s="21">
+        <f>M6*M5</f>
+        <v>12000000</v>
+      </c>
+      <c r="N7" s="21">
+        <f t="shared" ref="N7:Q7" si="1">N6*N5</f>
+        <v>13284000</v>
+      </c>
+      <c r="O7" s="21">
+        <f t="shared" si="1"/>
+        <v>14705388.000000002</v>
+      </c>
+      <c r="P7" s="21">
+        <f t="shared" si="1"/>
+        <v>16881785.424000002</v>
+      </c>
+      <c r="Q7" s="21">
+        <f t="shared" si="1"/>
+        <v>19380289.666752003</v>
+      </c>
+    </row>
+    <row r="9" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="K9" s="22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="K10" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="M10" s="21">
+        <v>-9000000</v>
+      </c>
+      <c r="N10" s="21">
+        <f>M10*(1+5%)</f>
+        <v>-9450000</v>
+      </c>
+      <c r="O10" s="21">
+        <f t="shared" ref="O10:Q10" si="2">N10*(1+5%)</f>
+        <v>-9922500</v>
+      </c>
+      <c r="P10" s="21">
+        <f t="shared" si="2"/>
+        <v>-10418625</v>
+      </c>
+      <c r="Q10" s="21">
+        <f t="shared" si="2"/>
+        <v>-10939556.25</v>
+      </c>
+    </row>
+    <row r="11" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="J11" s="21">
+        <v>-1000</v>
+      </c>
+      <c r="K11" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="M11" s="21">
+        <f>$J$11*M5*POWER(1.025,M3-1)</f>
+        <v>-1500000</v>
+      </c>
+      <c r="N11" s="21">
+        <f t="shared" ref="N11:Q11" si="3">$J$11*N5*POWER(1.025,N3-1)</f>
+        <v>-1660499.9999999998</v>
+      </c>
+      <c r="O11" s="21">
+        <f t="shared" si="3"/>
+        <v>-1838173.5</v>
+      </c>
+      <c r="P11" s="21">
+        <f t="shared" si="3"/>
+        <v>-2110223.1780000003</v>
+      </c>
+      <c r="Q11" s="21">
+        <f t="shared" si="3"/>
+        <v>-2422536.2083440004</v>
+      </c>
+    </row>
+    <row r="12" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="J12" s="21">
+        <f>-(2000000+1500000)/12</f>
+        <v>-291666.66666666669</v>
+      </c>
+      <c r="K12" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="M12" s="21">
+        <f>$J$12</f>
+        <v>-291666.66666666669</v>
+      </c>
+      <c r="N12" s="21">
+        <f t="shared" ref="N12:Q12" si="4">$J$12</f>
+        <v>-291666.66666666669</v>
+      </c>
+      <c r="O12" s="21">
+        <f t="shared" si="4"/>
+        <v>-291666.66666666669</v>
+      </c>
+      <c r="P12" s="21">
+        <f t="shared" si="4"/>
+        <v>-291666.66666666669</v>
+      </c>
+      <c r="Q12" s="21">
+        <f t="shared" si="4"/>
+        <v>-291666.66666666669</v>
+      </c>
+    </row>
+    <row r="13" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="K13" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="M13" s="21">
+        <v>-866333.70281249797</v>
+      </c>
+      <c r="N13" s="21">
+        <v>-748189.83712486597</v>
+      </c>
+      <c r="O13" s="21">
+        <v>-607301.07974262303</v>
+      </c>
+      <c r="P13" s="21">
+        <v>-439288.61594535602</v>
+      </c>
+      <c r="Q13" s="21">
+        <v>-238930.627730281</v>
+      </c>
+    </row>
+    <row r="14" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="K14" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="M14" s="21">
+        <f>-300000</f>
+        <v>-300000</v>
+      </c>
+      <c r="N14" s="21">
+        <f>M14*(1+2.5%)</f>
+        <v>-307500</v>
+      </c>
+      <c r="O14" s="21">
+        <f t="shared" ref="O14:Q14" si="5">N14*(1+2.5%)</f>
+        <v>-315187.5</v>
+      </c>
+      <c r="P14" s="21">
+        <f t="shared" si="5"/>
+        <v>-323067.1875</v>
+      </c>
+      <c r="Q14" s="21">
+        <f t="shared" si="5"/>
+        <v>-331143.8671875</v>
+      </c>
+    </row>
+    <row r="15" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="K15" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="M15" s="21">
+        <f>SUM(M10:M14)</f>
+        <v>-11958000.369479164</v>
+      </c>
+      <c r="N15" s="21">
+        <f t="shared" ref="N15:Q15" si="6">SUM(N10:N14)</f>
+        <v>-12457856.503791532</v>
+      </c>
+      <c r="O15" s="21">
+        <f t="shared" si="6"/>
+        <v>-12974828.74640929</v>
+      </c>
+      <c r="P15" s="21">
+        <f t="shared" si="6"/>
+        <v>-13582870.648112021</v>
+      </c>
+      <c r="Q15" s="21">
+        <f t="shared" si="6"/>
+        <v>-14223833.619928448</v>
+      </c>
+    </row>
+    <row r="16" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="K16" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="M16" s="21">
+        <f>M7+M15</f>
+        <v>41999.630520835519</v>
+      </c>
+      <c r="N16" s="21">
+        <f t="shared" ref="N16:Q16" si="7">N7+N15</f>
+        <v>826143.49620846845</v>
+      </c>
+      <c r="O16" s="21">
+        <f t="shared" si="7"/>
+        <v>1730559.2535907123</v>
+      </c>
+      <c r="P16" s="21">
+        <f t="shared" si="7"/>
+        <v>3298914.7758879811</v>
+      </c>
+      <c r="Q16" s="21">
+        <f t="shared" si="7"/>
+        <v>5156456.0468235556</v>
+      </c>
+    </row>
+    <row r="17" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="J17" s="23">
+        <v>-0.25</v>
+      </c>
+      <c r="K17" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="M17" s="21">
+        <f>$J$17*M16</f>
+        <v>-10499.90763020888</v>
+      </c>
+      <c r="N17" s="21">
+        <f t="shared" ref="N17:Q17" si="8">$J$17*N16</f>
+        <v>-206535.87405211711</v>
+      </c>
+      <c r="O17" s="21">
+        <f t="shared" si="8"/>
+        <v>-432639.81339767808</v>
+      </c>
+      <c r="P17" s="21">
+        <f t="shared" si="8"/>
+        <v>-824728.69397199526</v>
+      </c>
+      <c r="Q17" s="21">
+        <f t="shared" si="8"/>
+        <v>-1289114.0117058889</v>
+      </c>
+    </row>
+    <row r="19" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="K19" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="M19" s="21">
+        <f>M16+M17</f>
+        <v>31499.722890626639</v>
+      </c>
+      <c r="N19" s="21">
+        <f>N16+N17</f>
+        <v>619607.62215635134</v>
+      </c>
+      <c r="O19" s="21">
+        <f>O16+O17</f>
+        <v>1297919.4401930342</v>
+      </c>
+      <c r="P19" s="21">
+        <f>P16+P17</f>
+        <v>2474186.0819159858</v>
+      </c>
+      <c r="Q19" s="21">
+        <f>Q16+Q17</f>
+        <v>3867342.0351176667</v>
+      </c>
+    </row>
+    <row r="20" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="K20" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="M20" s="21">
+        <f>-M12</f>
+        <v>291666.66666666669</v>
+      </c>
+      <c r="N20" s="21">
+        <f t="shared" ref="N20:Q20" si="9">-N12</f>
+        <v>291666.66666666669</v>
+      </c>
+      <c r="O20" s="21">
+        <f t="shared" si="9"/>
+        <v>291666.66666666669</v>
+      </c>
+      <c r="P20" s="21">
+        <f t="shared" si="9"/>
+        <v>291666.66666666669</v>
+      </c>
+      <c r="Q20" s="21">
+        <f t="shared" si="9"/>
+        <v>291666.66666666669</v>
+      </c>
+    </row>
+    <row r="21" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="K21" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="M21" s="21">
+        <v>-613675.06985862798</v>
+      </c>
+      <c r="N21" s="21">
+        <v>-731818.93554625905</v>
+      </c>
+      <c r="O21" s="21">
+        <v>-872707.69292850199</v>
+      </c>
+      <c r="P21" s="21">
+        <v>-1040720.15672577</v>
+      </c>
+      <c r="Q21" s="21">
+        <v>-1241078.1449408401</v>
+      </c>
+    </row>
+    <row r="22" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="K22" s="22" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="K23" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="L23" s="21">
+        <v>-1000000</v>
+      </c>
+      <c r="Q23" s="21">
+        <f>-0.7*L23</f>
+        <v>700000</v>
+      </c>
+    </row>
+    <row r="24" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="K24" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="L24" s="21">
+        <v>-1500000</v>
+      </c>
+      <c r="Q24" s="21">
+        <f t="shared" ref="Q24:Q25" si="10">-0.7*L24</f>
+        <v>1050000</v>
+      </c>
+    </row>
+    <row r="25" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="K25" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="L25" s="21">
+        <v>-2000000</v>
+      </c>
+      <c r="Q25" s="21">
+        <f t="shared" si="10"/>
+        <v>1400000</v>
+      </c>
+    </row>
+    <row r="26" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="K26" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="L26" s="21">
+        <v>4500000</v>
+      </c>
+    </row>
+    <row r="27" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="K27" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="L27" s="21">
+        <f>1.5*M11</f>
+        <v>-2250000</v>
+      </c>
+      <c r="Q27" s="21">
+        <f>-0.85*L27</f>
+        <v>1912500</v>
+      </c>
+    </row>
+    <row r="28" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="K28" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="L28" s="21">
+        <f>SUM(L23:L27)</f>
+        <v>-2250000</v>
+      </c>
+      <c r="M28" s="21">
+        <f>SUM(M19:M27)</f>
+        <v>-290508.68030133465</v>
+      </c>
+      <c r="N28" s="21">
+        <f t="shared" ref="N28:Q28" si="11">SUM(N19:N27)</f>
+        <v>179455.35327675904</v>
+      </c>
+      <c r="O28" s="21">
+        <f t="shared" si="11"/>
+        <v>716878.413931199</v>
+      </c>
+      <c r="P28" s="21">
+        <f t="shared" si="11"/>
+        <v>1725132.5918568824</v>
+      </c>
+      <c r="Q28" s="21">
+        <f>SUM(Q19:Q27)</f>
+        <v>7980430.5568434931</v>
+      </c>
+    </row>
+    <row r="29" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="K29" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="L29" s="101">
+        <f>2%+1.2*10%</f>
+        <v>0.13999999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="K30" s="100" t="s">
+        <v>86</v>
+      </c>
+      <c r="L30" s="100">
+        <f>NPV(L29,M28:Q28)+L28</f>
+        <v>3283327.9442483895</v>
+      </c>
+    </row>
+    <row r="31" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="K31" s="100" t="s">
+        <v>88</v>
+      </c>
+      <c r="L31" s="102">
+        <f>IRR(L28:Q28)</f>
+        <v>0.3770042029363736</v>
+      </c>
+    </row>
+    <row r="33" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K33" s="98" t="s">
+        <v>6</v>
+      </c>
+      <c r="L33" s="99">
+        <f>POWER(1+(0.18/4),4)-1</f>
+        <v>0.19251860062499948</v>
+      </c>
+      <c r="M33" s="98" t="s">
+        <v>76</v>
+      </c>
+      <c r="N33" s="98">
+        <v>4500000</v>
+      </c>
+    </row>
+    <row r="34" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K34" s="98" t="s">
+        <v>7</v>
+      </c>
+      <c r="L34" s="98">
+        <f>-PMT(L33,5,N33)</f>
+        <v>1480008.7726711251</v>
+      </c>
+      <c r="M34" s="98"/>
+      <c r="N34" s="98"/>
+    </row>
+    <row r="35" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K35" s="98"/>
+      <c r="L35" s="98"/>
+      <c r="M35" s="98"/>
+      <c r="N35" s="98" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K36" s="98" t="s">
+        <v>6</v>
+      </c>
+      <c r="L36" s="98" t="s">
+        <v>7</v>
+      </c>
+      <c r="M36" s="98" t="s">
+        <v>8</v>
+      </c>
+      <c r="N36" s="98">
+        <f>N33</f>
+        <v>4500000</v>
+      </c>
+    </row>
+    <row r="37" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K37" s="98">
+        <f>$L$33*N36</f>
+        <v>866333.70281249762</v>
+      </c>
+      <c r="L37" s="98">
+        <f>$L$34</f>
+        <v>1480008.7726711251</v>
+      </c>
+      <c r="M37" s="98">
+        <f>L37-K37</f>
+        <v>613675.06985862751</v>
+      </c>
+      <c r="N37" s="98">
+        <f>N36-M37</f>
+        <v>3886324.9301413726</v>
+      </c>
+    </row>
+    <row r="38" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K38" s="98">
+        <f>$L$33*N37</f>
+        <v>748189.83712486597</v>
+      </c>
+      <c r="L38" s="98">
+        <f>$L$34</f>
+        <v>1480008.7726711251</v>
+      </c>
+      <c r="M38" s="98">
+        <f t="shared" ref="M38:M41" si="12">L38-K38</f>
+        <v>731818.93554625916</v>
+      </c>
+      <c r="N38" s="98">
+        <f t="shared" ref="N38:N41" si="13">N37-M38</f>
+        <v>3154505.9945951132</v>
+      </c>
+    </row>
+    <row r="39" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K39" s="98">
+        <f>$L$33*N38</f>
+        <v>607301.07974262338</v>
+      </c>
+      <c r="L39" s="98">
+        <f>$L$34</f>
+        <v>1480008.7726711251</v>
+      </c>
+      <c r="M39" s="98">
+        <f t="shared" si="12"/>
+        <v>872707.69292850175</v>
+      </c>
+      <c r="N39" s="98">
+        <f t="shared" si="13"/>
+        <v>2281798.3016666113</v>
+      </c>
+    </row>
+    <row r="40" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K40" s="98">
+        <f>$L$33*N39</f>
+        <v>439288.61594535643</v>
+      </c>
+      <c r="L40" s="98">
+        <f>$L$34</f>
+        <v>1480008.7726711251</v>
+      </c>
+      <c r="M40" s="98">
+        <f t="shared" si="12"/>
+        <v>1040720.1567257687</v>
+      </c>
+      <c r="N40" s="98">
+        <f t="shared" si="13"/>
+        <v>1241078.1449408426</v>
+      </c>
+    </row>
+    <row r="41" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K41" s="98">
+        <f>$L$33*N40</f>
+        <v>238930.6277302813</v>
+      </c>
+      <c r="L41" s="98">
+        <f>$L$34</f>
+        <v>1480008.7726711251</v>
+      </c>
+      <c r="M41" s="98">
+        <f t="shared" si="12"/>
+        <v>1241078.1449408438</v>
+      </c>
+      <c r="N41" s="98">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20AFEFDD-6C52-4CB7-9443-2E3596023181}">
+  <dimension ref="A3:W54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="97" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="96"/>
+      <c r="C4" s="96"/>
+      <c r="D4" s="96"/>
+      <c r="E4" s="96"/>
+      <c r="F4" s="96"/>
+      <c r="G4" s="96"/>
+      <c r="H4" s="96"/>
+      <c r="I4" s="96"/>
+      <c r="J4" s="96"/>
+      <c r="K4" s="96"/>
+      <c r="L4" s="96"/>
+      <c r="M4" s="96"/>
+      <c r="N4" s="96"/>
+      <c r="O4" s="96"/>
+      <c r="P4" s="96"/>
+      <c r="Q4" s="96"/>
+      <c r="R4" s="96"/>
+      <c r="S4" s="96"/>
+      <c r="T4" s="96"/>
+      <c r="U4" s="96"/>
+      <c r="V4" s="96"/>
+      <c r="W4" s="95"/>
+    </row>
+    <row r="5" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="94"/>
+      <c r="B5" s="93"/>
+      <c r="C5" s="93"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="93"/>
+      <c r="F5" s="93"/>
+      <c r="G5" s="93"/>
+      <c r="H5" s="93"/>
+      <c r="I5" s="93"/>
+      <c r="J5" s="93"/>
+      <c r="K5" s="93"/>
+      <c r="L5" s="93"/>
+      <c r="M5" s="93"/>
+      <c r="N5" s="93"/>
+      <c r="O5" s="93"/>
+      <c r="P5" s="93"/>
+      <c r="Q5" s="93"/>
+      <c r="R5" s="93"/>
+      <c r="S5" s="93"/>
+      <c r="T5" s="93"/>
+      <c r="U5" s="93"/>
+      <c r="V5" s="93"/>
+      <c r="W5" s="92"/>
+    </row>
+    <row r="6" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" s="50" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="49"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="45"/>
+      <c r="H7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" s="44"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="63" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="62" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="62" t="s">
+        <v>71</v>
+      </c>
+      <c r="G8" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="H8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="27">
+        <f>D9*POWER(1+E9,F9)</f>
+        <v>1628.8946267774415</v>
+      </c>
+      <c r="D9" s="57">
+        <v>1000</v>
+      </c>
+      <c r="E9" s="91">
+        <v>0.05</v>
+      </c>
+      <c r="F9" s="56">
+        <v>10</v>
+      </c>
+      <c r="G9" s="90">
+        <f>C9</f>
+        <v>1628.8946267774415</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" s="32"/>
+      <c r="B10" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="27">
+        <f>-FV(E9,F9,,D9)</f>
+        <v>1628.8946267774415</v>
+      </c>
+      <c r="D10" s="89"/>
+      <c r="E10" s="1"/>
+      <c r="G10" s="89"/>
+    </row>
+    <row r="11" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="88" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="27">
+        <f>-PV(E9,F9,,G9)</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="87"/>
+      <c r="B12" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="24">
+        <f>G9/POWER(1+E9,F9)</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A15" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="49"/>
+      <c r="C15" s="86" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="86"/>
+      <c r="E15" s="86"/>
+      <c r="F15" s="86"/>
+      <c r="G15" s="86"/>
+      <c r="H15" s="85"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16" s="44"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="84" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="84"/>
+      <c r="E16" s="84" t="s">
+        <v>65</v>
+      </c>
+      <c r="F16" s="84"/>
+      <c r="G16" s="84" t="s">
+        <v>64</v>
+      </c>
+      <c r="H16" s="83"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="82">
+        <f>POWER(1+(C17/F17),H17) -1</f>
+        <v>0.14999999999999991</v>
+      </c>
+      <c r="B17" s="81"/>
+      <c r="C17" s="80">
+        <v>0.15</v>
+      </c>
+      <c r="D17" s="80"/>
+      <c r="E17" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="F17" s="28">
+        <v>1</v>
+      </c>
+      <c r="G17" s="79" t="s">
+        <v>59</v>
+      </c>
+      <c r="H17" s="78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="82">
+        <f>POWER(1+(C18/F18),H18) -1</f>
+        <v>0</v>
+      </c>
+      <c r="B18" s="81"/>
+      <c r="C18" s="80">
+        <f>C17</f>
+        <v>0.15</v>
+      </c>
+      <c r="D18" s="80"/>
+      <c r="E18" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" s="28">
+        <v>1</v>
+      </c>
+      <c r="G18" s="79" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" s="78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="82">
+        <f>POWER(1+(C19/F19),H19) -1</f>
+        <v>0</v>
+      </c>
+      <c r="B19" s="81"/>
+      <c r="C19" s="80">
+        <f>C18</f>
+        <v>0.15</v>
+      </c>
+      <c r="D19" s="80"/>
+      <c r="E19" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" s="28">
+        <v>1</v>
+      </c>
+      <c r="G19" s="79" t="s">
+        <v>57</v>
+      </c>
+      <c r="H19" s="78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="82">
+        <f>POWER(1+(C20/F20),H20) -1</f>
+        <v>0</v>
+      </c>
+      <c r="B20" s="81"/>
+      <c r="C20" s="80">
+        <f>C19</f>
+        <v>0.15</v>
+      </c>
+      <c r="D20" s="80"/>
+      <c r="E20" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="F20" s="28">
+        <v>1</v>
+      </c>
+      <c r="G20" s="79" t="s">
+        <v>55</v>
+      </c>
+      <c r="H20" s="78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="82">
+        <f>POWER(1+(C21/F21),H21) -1</f>
+        <v>0.1556249999999999</v>
+      </c>
+      <c r="B21" s="81"/>
+      <c r="C21" s="80">
+        <f>C20</f>
+        <v>0.15</v>
+      </c>
+      <c r="D21" s="80"/>
+      <c r="E21" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="F21" s="28">
+        <v>2</v>
+      </c>
+      <c r="G21" s="79" t="s">
+        <v>59</v>
+      </c>
+      <c r="H21" s="78">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="82">
+        <f>POWER(1+(C22/F22),H22) -1</f>
+        <v>7.4999999999999956E-2</v>
+      </c>
+      <c r="B22" s="81"/>
+      <c r="C22" s="80">
+        <f>C21</f>
+        <v>0.15</v>
+      </c>
+      <c r="D22" s="80"/>
+      <c r="E22" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="F22" s="28">
+        <v>2</v>
+      </c>
+      <c r="G22" s="79" t="s">
+        <v>58</v>
+      </c>
+      <c r="H22" s="78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="82">
+        <f>POWER(1+(C23/F23),H23) -1</f>
+        <v>0</v>
+      </c>
+      <c r="B23" s="81"/>
+      <c r="C23" s="80">
+        <f>C22</f>
+        <v>0.15</v>
+      </c>
+      <c r="D23" s="80"/>
+      <c r="E23" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="F23" s="28">
+        <v>2</v>
+      </c>
+      <c r="G23" s="79" t="s">
+        <v>57</v>
+      </c>
+      <c r="H23" s="78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="82">
+        <f>POWER(1+(C24/F24),H24) -1</f>
+        <v>0</v>
+      </c>
+      <c r="B24" s="81"/>
+      <c r="C24" s="80">
+        <f>C23</f>
+        <v>0.15</v>
+      </c>
+      <c r="D24" s="80"/>
+      <c r="E24" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="F24" s="28">
+        <v>2</v>
+      </c>
+      <c r="G24" s="79" t="s">
+        <v>55</v>
+      </c>
+      <c r="H24" s="78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="82">
+        <f>POWER(1+(C25/F25),H25) -1</f>
+        <v>0.15865041503906308</v>
+      </c>
+      <c r="B25" s="81"/>
+      <c r="C25" s="80">
+        <f>C24</f>
+        <v>0.15</v>
+      </c>
+      <c r="D25" s="80"/>
+      <c r="E25" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="F25" s="28">
+        <v>4</v>
+      </c>
+      <c r="G25" s="79" t="s">
+        <v>59</v>
+      </c>
+      <c r="H25" s="78">
+        <v>4</v>
+      </c>
+      <c r="L25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="82">
+        <f>POWER(1+(C26/F26),H26) -1</f>
+        <v>7.6406250000000231E-2</v>
+      </c>
+      <c r="B26" s="81"/>
+      <c r="C26" s="80">
+        <f>C25</f>
+        <v>0.15</v>
+      </c>
+      <c r="D26" s="80"/>
+      <c r="E26" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="F26" s="28">
+        <v>4</v>
+      </c>
+      <c r="G26" s="79" t="s">
+        <v>58</v>
+      </c>
+      <c r="H26" s="78">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="82">
+        <f>POWER(1+(C27/F27),H27) -1</f>
+        <v>3.7500000000000089E-2</v>
+      </c>
+      <c r="B27" s="81"/>
+      <c r="C27" s="80">
+        <f>C26</f>
+        <v>0.15</v>
+      </c>
+      <c r="D27" s="80"/>
+      <c r="E27" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="F27" s="28">
+        <v>4</v>
+      </c>
+      <c r="G27" s="79" t="s">
+        <v>57</v>
+      </c>
+      <c r="H27" s="78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="82">
+        <f>POWER(1+(C28/F28),H28) -1</f>
+        <v>0</v>
+      </c>
+      <c r="B28" s="81"/>
+      <c r="C28" s="80">
+        <f>C27</f>
+        <v>0.15</v>
+      </c>
+      <c r="D28" s="80"/>
+      <c r="E28" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="F28" s="28">
+        <v>4</v>
+      </c>
+      <c r="G28" s="79" t="s">
+        <v>55</v>
+      </c>
+      <c r="H28" s="78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="82">
+        <f>POWER(1+(C29/F29),H29) -1</f>
+        <v>0.16075451772299854</v>
+      </c>
+      <c r="B29" s="81"/>
+      <c r="C29" s="80">
+        <f>C28</f>
+        <v>0.15</v>
+      </c>
+      <c r="D29" s="80"/>
+      <c r="E29" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="F29" s="28">
+        <v>12</v>
+      </c>
+      <c r="G29" s="79" t="s">
+        <v>59</v>
+      </c>
+      <c r="H29" s="78">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="82">
+        <f>POWER(1+(C30/F30),H30) -1</f>
+        <v>7.7383180545806729E-2</v>
+      </c>
+      <c r="B30" s="81"/>
+      <c r="C30" s="80">
+        <f>C29</f>
+        <v>0.15</v>
+      </c>
+      <c r="D30" s="80"/>
+      <c r="E30" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" s="28">
+        <v>12</v>
+      </c>
+      <c r="G30" s="79" t="s">
+        <v>58</v>
+      </c>
+      <c r="H30" s="78">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="82">
+        <f>POWER(1+(C31/F31),H31) -1</f>
+        <v>3.7970703124999838E-2</v>
+      </c>
+      <c r="B31" s="81"/>
+      <c r="C31" s="80">
+        <f>C30</f>
+        <v>0.15</v>
+      </c>
+      <c r="D31" s="80"/>
+      <c r="E31" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="F31" s="28">
+        <v>12</v>
+      </c>
+      <c r="G31" s="79" t="s">
+        <v>57</v>
+      </c>
+      <c r="H31" s="78">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="77">
+        <f>POWER(1+(C32/F32),H32) -1</f>
+        <v>1.2499999999999956E-2</v>
+      </c>
+      <c r="B32" s="76"/>
+      <c r="C32" s="75">
+        <f>C31</f>
+        <v>0.15</v>
+      </c>
+      <c r="D32" s="75"/>
+      <c r="E32" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="F32" s="25">
+        <v>12</v>
+      </c>
+      <c r="G32" s="74" t="s">
+        <v>55</v>
+      </c>
+      <c r="H32" s="73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" s="49"/>
+      <c r="C38" s="48"/>
+      <c r="D38" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="E38" s="68"/>
+      <c r="F38" s="68"/>
+      <c r="G38" s="67"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="44"/>
+      <c r="B39" s="43"/>
+      <c r="C39" s="42"/>
+      <c r="D39" s="63" t="s">
+        <v>53</v>
+      </c>
+      <c r="E39" s="62" t="s">
+        <v>19</v>
+      </c>
+      <c r="F39" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="G39" s="61"/>
+    </row>
+    <row r="40" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="60" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" s="59">
+        <f>-PMT(F40,E40,D40)</f>
+        <v>11379731.896831043</v>
+      </c>
+      <c r="C40" s="58"/>
+      <c r="D40" s="57">
+        <v>65000000</v>
+      </c>
+      <c r="E40" s="56">
+        <v>8</v>
+      </c>
+      <c r="F40" s="55">
+        <v>8.1600000000000006E-2</v>
+      </c>
+      <c r="G40" s="54"/>
+    </row>
+    <row r="41" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="52">
+        <f>D40*(F40*POWER(1+F40,E40)/(POWER(1+F40,E40)-1))</f>
+        <v>11379731.896831054</v>
+      </c>
+      <c r="C41" s="51"/>
+    </row>
+    <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="71" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43" s="70"/>
+      <c r="C43" s="69"/>
+      <c r="D43" s="68" t="s">
+        <v>49</v>
+      </c>
+      <c r="E43" s="68"/>
+      <c r="F43" s="68"/>
+      <c r="G43" s="67"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="66"/>
+      <c r="B44" s="65"/>
+      <c r="C44" s="64"/>
+      <c r="D44" s="63" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" s="62" t="s">
+        <v>19</v>
+      </c>
+      <c r="F44" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="G44" s="61"/>
+    </row>
+    <row r="45" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="60" t="s">
+        <v>42</v>
+      </c>
+      <c r="B45" s="59">
+        <f>-PV(F45,E45,D45)</f>
+        <v>294.03131444078036</v>
+      </c>
+      <c r="C45" s="58"/>
+      <c r="D45" s="57">
+        <v>110</v>
+      </c>
+      <c r="E45" s="56">
+        <v>3</v>
+      </c>
+      <c r="F45" s="55">
+        <v>0.06</v>
+      </c>
+      <c r="G45" s="54"/>
+    </row>
+    <row r="46" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="B46" s="52">
+        <f>D45*((POWER(1+F45,E45)-1)/(F45*POWER(1+F45,E45)))</f>
+        <v>294.03131444078036</v>
+      </c>
+      <c r="C46" s="51"/>
+    </row>
+    <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A49" s="50" t="s">
+        <v>50</v>
+      </c>
+      <c r="B49" s="49"/>
+      <c r="C49" s="48"/>
+      <c r="D49" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="E49" s="46"/>
+      <c r="F49" s="46"/>
+      <c r="G49" s="46"/>
+      <c r="H49" s="45"/>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A50" s="44"/>
+      <c r="B50" s="43"/>
+      <c r="C50" s="42"/>
+      <c r="D50" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="E50" s="40"/>
+      <c r="F50" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="G50" s="40"/>
+      <c r="H50" s="39" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="B51" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="C51" s="37">
+        <f>D51*F51*H51</f>
+        <v>1357350.3</v>
+      </c>
+      <c r="D51" s="36">
+        <v>45245010</v>
+      </c>
+      <c r="E51" s="34"/>
+      <c r="F51" s="35">
+        <v>0.01</v>
+      </c>
+      <c r="G51" s="34"/>
+      <c r="H51" s="33">
+        <v>3</v>
+      </c>
+      <c r="O51" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A52" s="32"/>
+      <c r="B52" s="31"/>
+      <c r="C52" s="30"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="20"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A53" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B53" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="C53" s="27">
+        <f>D51*(POWER(1+F51,H51)-1)</f>
+        <v>1370969.0480099961</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="26"/>
+      <c r="B54" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C54" s="24">
+        <f>-FV(F51,H51,,D51)-D51</f>
+        <v>1370969.0480099991</v>
+      </c>
+      <c r="O54" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="65">
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="A49:C50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="A43:C44"/>
+    <mergeCell ref="D43:G43"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="D49:H49"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="D38:G38"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="A38:C39"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="A15:B16"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="A7:C8"/>
+    <mergeCell ref="A4:W5"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
vault backup: 2024-10-01 00:30:22
</commit_message>
<xml_diff>
--- a/2024-2/Evaluación de proyectos/Excels/Ejercicios_sol_1.xlsx
+++ b/2024-2/Evaluación de proyectos/Excels/Ejercicios_sol_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IVAN\Desktop\Codes\Apuntes_2024\2024-2\Evaluación de proyectos\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF3F871-6C4B-4D31-8E1E-08EA24E03523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FB8760-9455-421B-AEDB-1EE0D9119A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{C81B0A03-BDB8-4836-9CA0-B318B652DAA5}"/>
+    <workbookView xWindow="1740" yWindow="990" windowWidth="26100" windowHeight="14100" activeTab="2" xr2:uid="{C81B0A03-BDB8-4836-9CA0-B318B652DAA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Ej Aprovación de credito" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -323,7 +323,7 @@
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;\-#,##0.00"/>
     <numFmt numFmtId="42" formatCode="_ &quot;$&quot;* #,##0_ ;_ &quot;$&quot;* \-#,##0_ ;_ &quot;$&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;$&quot;* #,##0.00_ ;_ &quot;$&quot;* \-#,##0.00_ ;_ &quot;$&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="168" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -764,7 +764,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -782,221 +782,220 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="6" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="6" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="3" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="3" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moneda [0]" xfId="1" builtinId="7"/>
@@ -2511,7 +2510,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C56BEC62-8017-431D-B3BC-C82E605B6596}" name="TablaDinámica1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C56BEC62-8017-431D-B3BC-C82E605B6596}" name="TablaDinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="H4:I7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -2874,8 +2873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16A51246-93CB-4F0A-B41E-2FA7CB8E0C7A}">
   <dimension ref="F2:K44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3094,12 +3093,12 @@
       </c>
     </row>
     <row r="18" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G18" s="15" t="s">
+      <c r="G18" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G19" s="2" t="s">
@@ -3124,17 +3123,17 @@
       <c r="J20" s="2"/>
     </row>
     <row r="22" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G22" s="16" t="s">
+      <c r="G22" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="H22" s="17"/>
+      <c r="H22" s="44"/>
     </row>
     <row r="23" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G23" s="18">
+      <c r="G23" s="45">
         <f>K13-I20</f>
         <v>1584195.701267676</v>
       </c>
-      <c r="H23" s="19"/>
+      <c r="H23" s="46"/>
     </row>
     <row r="24" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G24" s="2" t="s">
@@ -3250,7 +3249,7 @@
         <v>20</v>
       </c>
       <c r="I34" s="1">
-        <v>1.03</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="35" spans="7:9" x14ac:dyDescent="0.25">
@@ -3271,8 +3270,8 @@
       <c r="H36" s="5">
         <v>2107535.6902545234</v>
       </c>
-      <c r="I36" s="9">
-        <f>H36/($I$34^G36)</f>
+      <c r="I36" s="6">
+        <f>-PV($I$34,G36,,H36)</f>
         <v>2046151.1555869158</v>
       </c>
     </row>
@@ -3283,8 +3282,8 @@
       <c r="H37" s="5">
         <v>2107535.6902545234</v>
       </c>
-      <c r="I37" s="9">
-        <f t="shared" ref="I37:I42" si="7">H37/($I$34^G37)</f>
+      <c r="I37" s="6">
+        <f t="shared" ref="I37:I42" si="7">-PV($I$34,G37,,H37)</f>
         <v>1986554.519987297</v>
       </c>
     </row>
@@ -3295,7 +3294,7 @@
       <c r="H38" s="5">
         <v>2107535.6902545234</v>
       </c>
-      <c r="I38" s="9">
+      <c r="I38" s="6">
         <f t="shared" si="7"/>
         <v>1928693.7087255311</v>
       </c>
@@ -3307,7 +3306,7 @@
       <c r="H39" s="5">
         <v>2107535.6902545234</v>
       </c>
-      <c r="I39" s="9">
+      <c r="I39" s="6">
         <f t="shared" si="7"/>
         <v>1872518.1638111954</v>
       </c>
@@ -3319,7 +3318,7 @@
       <c r="H40" s="5">
         <v>614721.02489998355</v>
       </c>
-      <c r="I40" s="9">
+      <c r="I40" s="6">
         <f t="shared" si="7"/>
         <v>530263.75602436229</v>
       </c>
@@ -3331,7 +3330,7 @@
       <c r="H41" s="5">
         <v>614721.02489998355</v>
       </c>
-      <c r="I41" s="9">
+      <c r="I41" s="6">
         <f t="shared" si="7"/>
         <v>514819.18060617696</v>
       </c>
@@ -3343,16 +3342,16 @@
       <c r="H42" s="5">
         <v>614721.02489998355</v>
       </c>
-      <c r="I42" s="9">
+      <c r="I42" s="6">
         <f t="shared" si="7"/>
         <v>499824.44719046302</v>
       </c>
     </row>
     <row r="44" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G44" s="20" t="s">
+      <c r="G44" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="H44" s="20"/>
+      <c r="H44" s="47"/>
       <c r="I44" s="7">
         <f>SUM(I36:I42)</f>
         <v>9378824.9319319427</v>
@@ -3433,7 +3432,7 @@
       <c r="H5" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="103">
+      <c r="I5">
         <v>1709</v>
       </c>
     </row>
@@ -3451,7 +3450,7 @@
       <c r="H6" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="I6" s="103">
+      <c r="I6">
         <v>12787</v>
       </c>
     </row>
@@ -3469,7 +3468,7 @@
       <c r="H7" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="I7" s="103">
+      <c r="I7">
         <v>14496</v>
       </c>
     </row>
@@ -3694,646 +3693,646 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C8269A2-8272-4B58-BB60-2DE0A7F360FB}">
   <dimension ref="J3:Q41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="10" width="11.42578125" style="21"/>
-    <col min="11" max="11" width="27" style="21" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" style="21"/>
-    <col min="13" max="13" width="14.5703125" style="21" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="11.42578125" style="21"/>
+    <col min="1" max="10" width="11.42578125" style="15"/>
+    <col min="11" max="11" width="27" style="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" style="15"/>
+    <col min="13" max="13" width="14.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="11.42578125" style="15"/>
   </cols>
   <sheetData>
     <row r="3" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="M3" s="21">
+      <c r="M3" s="15">
         <v>1</v>
       </c>
-      <c r="N3" s="21">
+      <c r="N3" s="15">
         <v>2</v>
       </c>
-      <c r="O3" s="21">
+      <c r="O3" s="15">
         <v>3</v>
       </c>
-      <c r="P3" s="21">
+      <c r="P3" s="15">
         <v>4</v>
       </c>
-      <c r="Q3" s="21">
+      <c r="Q3" s="15">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="K4" s="22" t="s">
+      <c r="K4" s="16" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="K5" s="21" t="s">
+      <c r="K5" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="M5" s="21">
+      <c r="M5" s="15">
         <v>1500</v>
       </c>
-      <c r="N5" s="21">
+      <c r="N5" s="15">
         <f>M5*(1+8%)</f>
         <v>1620</v>
       </c>
-      <c r="O5" s="21">
+      <c r="O5" s="15">
         <f>N5*(1+8%)</f>
         <v>1749.6000000000001</v>
       </c>
-      <c r="P5" s="21">
+      <c r="P5" s="15">
         <f>O5*(1+12%)</f>
         <v>1959.5520000000004</v>
       </c>
-      <c r="Q5" s="21">
+      <c r="Q5" s="15">
         <f>P5*(1+12%)</f>
         <v>2194.6982400000006</v>
       </c>
     </row>
     <row r="6" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="K6" s="21" t="s">
+      <c r="K6" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="M6" s="21">
+      <c r="M6" s="15">
         <v>8000</v>
       </c>
-      <c r="N6" s="21">
+      <c r="N6" s="15">
         <f>M6*(1+2.5%)</f>
         <v>8200</v>
       </c>
-      <c r="O6" s="21">
+      <c r="O6" s="15">
         <f t="shared" ref="O6:Q6" si="0">N6*(1+2.5%)</f>
         <v>8405</v>
       </c>
-      <c r="P6" s="21">
+      <c r="P6" s="15">
         <f t="shared" si="0"/>
         <v>8615.125</v>
       </c>
-      <c r="Q6" s="21">
+      <c r="Q6" s="15">
         <f t="shared" si="0"/>
         <v>8830.5031249999993</v>
       </c>
     </row>
     <row r="7" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="K7" s="21" t="s">
+      <c r="K7" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="M7" s="21">
+      <c r="M7" s="15">
         <f>M6*M5</f>
         <v>12000000</v>
       </c>
-      <c r="N7" s="21">
+      <c r="N7" s="15">
         <f t="shared" ref="N7:Q7" si="1">N6*N5</f>
         <v>13284000</v>
       </c>
-      <c r="O7" s="21">
+      <c r="O7" s="15">
         <f t="shared" si="1"/>
         <v>14705388.000000002</v>
       </c>
-      <c r="P7" s="21">
+      <c r="P7" s="15">
         <f t="shared" si="1"/>
         <v>16881785.424000002</v>
       </c>
-      <c r="Q7" s="21">
+      <c r="Q7" s="15">
         <f t="shared" si="1"/>
         <v>19380289.666752003</v>
       </c>
     </row>
     <row r="9" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="K9" s="22" t="s">
+      <c r="K9" s="16" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="10" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="K10" s="21" t="s">
+      <c r="K10" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="M10" s="21">
+      <c r="M10" s="15">
         <v>-9000000</v>
       </c>
-      <c r="N10" s="21">
+      <c r="N10" s="15">
         <f>M10*(1+5%)</f>
         <v>-9450000</v>
       </c>
-      <c r="O10" s="21">
+      <c r="O10" s="15">
         <f t="shared" ref="O10:Q10" si="2">N10*(1+5%)</f>
         <v>-9922500</v>
       </c>
-      <c r="P10" s="21">
+      <c r="P10" s="15">
         <f t="shared" si="2"/>
         <v>-10418625</v>
       </c>
-      <c r="Q10" s="21">
+      <c r="Q10" s="15">
         <f t="shared" si="2"/>
         <v>-10939556.25</v>
       </c>
     </row>
     <row r="11" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J11" s="21">
+      <c r="J11" s="15">
         <v>-1000</v>
       </c>
-      <c r="K11" s="21" t="s">
+      <c r="K11" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="M11" s="21">
+      <c r="M11" s="15">
         <f>$J$11*M5*POWER(1.025,M3-1)</f>
         <v>-1500000</v>
       </c>
-      <c r="N11" s="21">
+      <c r="N11" s="15">
         <f t="shared" ref="N11:Q11" si="3">$J$11*N5*POWER(1.025,N3-1)</f>
         <v>-1660499.9999999998</v>
       </c>
-      <c r="O11" s="21">
+      <c r="O11" s="15">
         <f t="shared" si="3"/>
         <v>-1838173.5</v>
       </c>
-      <c r="P11" s="21">
+      <c r="P11" s="15">
         <f t="shared" si="3"/>
         <v>-2110223.1780000003</v>
       </c>
-      <c r="Q11" s="21">
+      <c r="Q11" s="15">
         <f t="shared" si="3"/>
         <v>-2422536.2083440004</v>
       </c>
     </row>
     <row r="12" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J12" s="21">
+      <c r="J12" s="15">
         <f>-(2000000+1500000)/12</f>
         <v>-291666.66666666669</v>
       </c>
-      <c r="K12" s="21" t="s">
+      <c r="K12" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="M12" s="21">
+      <c r="M12" s="15">
         <f>$J$12</f>
         <v>-291666.66666666669</v>
       </c>
-      <c r="N12" s="21">
+      <c r="N12" s="15">
         <f t="shared" ref="N12:Q12" si="4">$J$12</f>
         <v>-291666.66666666669</v>
       </c>
-      <c r="O12" s="21">
+      <c r="O12" s="15">
         <f t="shared" si="4"/>
         <v>-291666.66666666669</v>
       </c>
-      <c r="P12" s="21">
+      <c r="P12" s="15">
         <f t="shared" si="4"/>
         <v>-291666.66666666669</v>
       </c>
-      <c r="Q12" s="21">
+      <c r="Q12" s="15">
         <f t="shared" si="4"/>
         <v>-291666.66666666669</v>
       </c>
     </row>
     <row r="13" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="K13" s="21" t="s">
+      <c r="K13" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="M13" s="21">
+      <c r="M13" s="15">
         <v>-866333.70281249797</v>
       </c>
-      <c r="N13" s="21">
+      <c r="N13" s="15">
         <v>-748189.83712486597</v>
       </c>
-      <c r="O13" s="21">
+      <c r="O13" s="15">
         <v>-607301.07974262303</v>
       </c>
-      <c r="P13" s="21">
+      <c r="P13" s="15">
         <v>-439288.61594535602</v>
       </c>
-      <c r="Q13" s="21">
+      <c r="Q13" s="15">
         <v>-238930.627730281</v>
       </c>
     </row>
     <row r="14" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="K14" s="21" t="s">
+      <c r="K14" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="M14" s="21">
+      <c r="M14" s="15">
         <f>-300000</f>
         <v>-300000</v>
       </c>
-      <c r="N14" s="21">
+      <c r="N14" s="15">
         <f>M14*(1+2.5%)</f>
         <v>-307500</v>
       </c>
-      <c r="O14" s="21">
+      <c r="O14" s="15">
         <f t="shared" ref="O14:Q14" si="5">N14*(1+2.5%)</f>
         <v>-315187.5</v>
       </c>
-      <c r="P14" s="21">
+      <c r="P14" s="15">
         <f t="shared" si="5"/>
         <v>-323067.1875</v>
       </c>
-      <c r="Q14" s="21">
+      <c r="Q14" s="15">
         <f t="shared" si="5"/>
         <v>-331143.8671875</v>
       </c>
     </row>
     <row r="15" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="K15" s="21" t="s">
+      <c r="K15" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="M15" s="21">
+      <c r="M15" s="15">
         <f>SUM(M10:M14)</f>
         <v>-11958000.369479164</v>
       </c>
-      <c r="N15" s="21">
+      <c r="N15" s="15">
         <f t="shared" ref="N15:Q15" si="6">SUM(N10:N14)</f>
         <v>-12457856.503791532</v>
       </c>
-      <c r="O15" s="21">
+      <c r="O15" s="15">
         <f t="shared" si="6"/>
         <v>-12974828.74640929</v>
       </c>
-      <c r="P15" s="21">
+      <c r="P15" s="15">
         <f t="shared" si="6"/>
         <v>-13582870.648112021</v>
       </c>
-      <c r="Q15" s="21">
+      <c r="Q15" s="15">
         <f t="shared" si="6"/>
         <v>-14223833.619928448</v>
       </c>
     </row>
     <row r="16" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="K16" s="21" t="s">
+      <c r="K16" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="M16" s="21">
+      <c r="M16" s="15">
         <f>M7+M15</f>
         <v>41999.630520835519</v>
       </c>
-      <c r="N16" s="21">
+      <c r="N16" s="15">
         <f t="shared" ref="N16:Q16" si="7">N7+N15</f>
         <v>826143.49620846845</v>
       </c>
-      <c r="O16" s="21">
+      <c r="O16" s="15">
         <f t="shared" si="7"/>
         <v>1730559.2535907123</v>
       </c>
-      <c r="P16" s="21">
+      <c r="P16" s="15">
         <f t="shared" si="7"/>
         <v>3298914.7758879811</v>
       </c>
-      <c r="Q16" s="21">
+      <c r="Q16" s="15">
         <f t="shared" si="7"/>
         <v>5156456.0468235556</v>
       </c>
     </row>
     <row r="17" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J17" s="23">
+      <c r="J17" s="17">
         <v>-0.25</v>
       </c>
-      <c r="K17" s="21" t="s">
+      <c r="K17" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="M17" s="21">
+      <c r="M17" s="15">
         <f>$J$17*M16</f>
         <v>-10499.90763020888</v>
       </c>
-      <c r="N17" s="21">
+      <c r="N17" s="15">
         <f t="shared" ref="N17:Q17" si="8">$J$17*N16</f>
         <v>-206535.87405211711</v>
       </c>
-      <c r="O17" s="21">
+      <c r="O17" s="15">
         <f t="shared" si="8"/>
         <v>-432639.81339767808</v>
       </c>
-      <c r="P17" s="21">
+      <c r="P17" s="15">
         <f t="shared" si="8"/>
         <v>-824728.69397199526</v>
       </c>
-      <c r="Q17" s="21">
+      <c r="Q17" s="15">
         <f t="shared" si="8"/>
         <v>-1289114.0117058889</v>
       </c>
     </row>
     <row r="19" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="K19" s="22" t="s">
+      <c r="K19" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="M19" s="21">
+      <c r="M19" s="15">
         <f>M16+M17</f>
         <v>31499.722890626639</v>
       </c>
-      <c r="N19" s="21">
+      <c r="N19" s="15">
         <f>N16+N17</f>
         <v>619607.62215635134</v>
       </c>
-      <c r="O19" s="21">
+      <c r="O19" s="15">
         <f>O16+O17</f>
         <v>1297919.4401930342</v>
       </c>
-      <c r="P19" s="21">
+      <c r="P19" s="15">
         <f>P16+P17</f>
         <v>2474186.0819159858</v>
       </c>
-      <c r="Q19" s="21">
+      <c r="Q19" s="15">
         <f>Q16+Q17</f>
         <v>3867342.0351176667</v>
       </c>
     </row>
     <row r="20" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="K20" s="21" t="s">
+      <c r="K20" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="M20" s="21">
+      <c r="M20" s="15">
         <f>-M12</f>
         <v>291666.66666666669</v>
       </c>
-      <c r="N20" s="21">
+      <c r="N20" s="15">
         <f t="shared" ref="N20:Q20" si="9">-N12</f>
         <v>291666.66666666669</v>
       </c>
-      <c r="O20" s="21">
+      <c r="O20" s="15">
         <f t="shared" si="9"/>
         <v>291666.66666666669</v>
       </c>
-      <c r="P20" s="21">
+      <c r="P20" s="15">
         <f t="shared" si="9"/>
         <v>291666.66666666669</v>
       </c>
-      <c r="Q20" s="21">
+      <c r="Q20" s="15">
         <f t="shared" si="9"/>
         <v>291666.66666666669</v>
       </c>
     </row>
     <row r="21" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="K21" s="21" t="s">
+      <c r="K21" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="M21" s="21">
+      <c r="M21" s="15">
         <v>-613675.06985862798</v>
       </c>
-      <c r="N21" s="21">
+      <c r="N21" s="15">
         <v>-731818.93554625905</v>
       </c>
-      <c r="O21" s="21">
+      <c r="O21" s="15">
         <v>-872707.69292850199</v>
       </c>
-      <c r="P21" s="21">
+      <c r="P21" s="15">
         <v>-1040720.15672577</v>
       </c>
-      <c r="Q21" s="21">
+      <c r="Q21" s="15">
         <v>-1241078.1449408401</v>
       </c>
     </row>
     <row r="22" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="K22" s="22" t="s">
+      <c r="K22" s="16" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="23" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="K23" s="21" t="s">
+      <c r="K23" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="L23" s="21">
+      <c r="L23" s="15">
         <v>-1000000</v>
       </c>
-      <c r="Q23" s="21">
+      <c r="Q23" s="15">
         <f>-0.7*L23</f>
         <v>700000</v>
       </c>
     </row>
     <row r="24" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="K24" s="21" t="s">
+      <c r="K24" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="L24" s="21">
+      <c r="L24" s="15">
         <v>-1500000</v>
       </c>
-      <c r="Q24" s="21">
+      <c r="Q24" s="15">
         <f t="shared" ref="Q24:Q25" si="10">-0.7*L24</f>
         <v>1050000</v>
       </c>
     </row>
     <row r="25" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="K25" s="21" t="s">
+      <c r="K25" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="L25" s="21">
+      <c r="L25" s="15">
         <v>-2000000</v>
       </c>
-      <c r="Q25" s="21">
+      <c r="Q25" s="15">
         <f t="shared" si="10"/>
         <v>1400000</v>
       </c>
     </row>
     <row r="26" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="K26" s="21" t="s">
+      <c r="K26" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="L26" s="21">
+      <c r="L26" s="15">
         <v>4500000</v>
       </c>
     </row>
     <row r="27" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="K27" s="21" t="s">
+      <c r="K27" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="L27" s="21">
+      <c r="L27" s="15">
         <f>1.5*M11</f>
         <v>-2250000</v>
       </c>
-      <c r="Q27" s="21">
+      <c r="Q27" s="15">
         <f>-0.85*L27</f>
         <v>1912500</v>
       </c>
     </row>
     <row r="28" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="K28" s="21" t="s">
+      <c r="K28" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="L28" s="21">
+      <c r="L28" s="15">
         <f>SUM(L23:L27)</f>
         <v>-2250000</v>
       </c>
-      <c r="M28" s="21">
+      <c r="M28" s="15">
         <f>SUM(M19:M27)</f>
         <v>-290508.68030133465</v>
       </c>
-      <c r="N28" s="21">
-        <f t="shared" ref="N28:Q28" si="11">SUM(N19:N27)</f>
+      <c r="N28" s="15">
+        <f t="shared" ref="N28:P28" si="11">SUM(N19:N27)</f>
         <v>179455.35327675904</v>
       </c>
-      <c r="O28" s="21">
+      <c r="O28" s="15">
         <f t="shared" si="11"/>
         <v>716878.413931199</v>
       </c>
-      <c r="P28" s="21">
+      <c r="P28" s="15">
         <f t="shared" si="11"/>
         <v>1725132.5918568824</v>
       </c>
-      <c r="Q28" s="21">
+      <c r="Q28" s="15">
         <f>SUM(Q19:Q27)</f>
         <v>7980430.5568434931</v>
       </c>
     </row>
     <row r="29" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="K29" s="21" t="s">
+      <c r="K29" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="L29" s="101">
+      <c r="L29" s="40">
         <f>2%+1.2*10%</f>
         <v>0.13999999999999999</v>
       </c>
     </row>
     <row r="30" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="K30" s="100" t="s">
+      <c r="K30" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="L30" s="100">
+      <c r="L30" s="39">
         <f>NPV(L29,M28:Q28)+L28</f>
         <v>3283327.9442483895</v>
       </c>
     </row>
     <row r="31" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="K31" s="100" t="s">
+      <c r="K31" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="L31" s="102">
+      <c r="L31" s="41">
         <f>IRR(L28:Q28)</f>
         <v>0.3770042029363736</v>
       </c>
     </row>
     <row r="33" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K33" s="98" t="s">
+      <c r="K33" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="L33" s="99">
+      <c r="L33" s="38">
         <f>POWER(1+(0.18/4),4)-1</f>
         <v>0.19251860062499948</v>
       </c>
-      <c r="M33" s="98" t="s">
+      <c r="M33" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="N33" s="98">
+      <c r="N33" s="37">
         <v>4500000</v>
       </c>
     </row>
     <row r="34" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K34" s="98" t="s">
+      <c r="K34" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="L34" s="98">
+      <c r="L34" s="37">
         <f>-PMT(L33,5,N33)</f>
         <v>1480008.7726711251</v>
       </c>
-      <c r="M34" s="98"/>
-      <c r="N34" s="98"/>
+      <c r="M34" s="37"/>
+      <c r="N34" s="37"/>
     </row>
     <row r="35" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K35" s="98"/>
-      <c r="L35" s="98"/>
-      <c r="M35" s="98"/>
-      <c r="N35" s="98" t="s">
+      <c r="K35" s="37"/>
+      <c r="L35" s="37"/>
+      <c r="M35" s="37"/>
+      <c r="N35" s="37" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="36" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K36" s="98" t="s">
+      <c r="K36" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="L36" s="98" t="s">
+      <c r="L36" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="M36" s="98" t="s">
+      <c r="M36" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="N36" s="98">
+      <c r="N36" s="37">
         <f>N33</f>
         <v>4500000</v>
       </c>
     </row>
     <row r="37" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K37" s="98">
+      <c r="K37" s="37">
         <f>$L$33*N36</f>
         <v>866333.70281249762</v>
       </c>
-      <c r="L37" s="98">
+      <c r="L37" s="37">
         <f>$L$34</f>
         <v>1480008.7726711251</v>
       </c>
-      <c r="M37" s="98">
+      <c r="M37" s="37">
         <f>L37-K37</f>
         <v>613675.06985862751</v>
       </c>
-      <c r="N37" s="98">
+      <c r="N37" s="37">
         <f>N36-M37</f>
         <v>3886324.9301413726</v>
       </c>
     </row>
     <row r="38" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K38" s="98">
+      <c r="K38" s="37">
         <f>$L$33*N37</f>
         <v>748189.83712486597</v>
       </c>
-      <c r="L38" s="98">
+      <c r="L38" s="37">
         <f>$L$34</f>
         <v>1480008.7726711251</v>
       </c>
-      <c r="M38" s="98">
+      <c r="M38" s="37">
         <f t="shared" ref="M38:M41" si="12">L38-K38</f>
         <v>731818.93554625916</v>
       </c>
-      <c r="N38" s="98">
+      <c r="N38" s="37">
         <f t="shared" ref="N38:N41" si="13">N37-M38</f>
         <v>3154505.9945951132</v>
       </c>
     </row>
     <row r="39" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K39" s="98">
+      <c r="K39" s="37">
         <f>$L$33*N38</f>
         <v>607301.07974262338</v>
       </c>
-      <c r="L39" s="98">
+      <c r="L39" s="37">
         <f>$L$34</f>
         <v>1480008.7726711251</v>
       </c>
-      <c r="M39" s="98">
+      <c r="M39" s="37">
         <f t="shared" si="12"/>
         <v>872707.69292850175</v>
       </c>
-      <c r="N39" s="98">
+      <c r="N39" s="37">
         <f t="shared" si="13"/>
         <v>2281798.3016666113</v>
       </c>
     </row>
     <row r="40" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K40" s="98">
+      <c r="K40" s="37">
         <f>$L$33*N39</f>
         <v>439288.61594535643</v>
       </c>
-      <c r="L40" s="98">
+      <c r="L40" s="37">
         <f>$L$34</f>
         <v>1480008.7726711251</v>
       </c>
-      <c r="M40" s="98">
+      <c r="M40" s="37">
         <f t="shared" si="12"/>
         <v>1040720.1567257687</v>
       </c>
-      <c r="N40" s="98">
+      <c r="N40" s="37">
         <f t="shared" si="13"/>
         <v>1241078.1449408426</v>
       </c>
     </row>
     <row r="41" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K41" s="98">
+      <c r="K41" s="37">
         <f>$L$33*N40</f>
         <v>238930.6277302813</v>
       </c>
-      <c r="L41" s="98">
+      <c r="L41" s="37">
         <f>$L$34</f>
         <v>1480008.7726711251</v>
       </c>
-      <c r="M41" s="98">
+      <c r="M41" s="37">
         <f t="shared" si="12"/>
         <v>1241078.1449408438</v>
       </c>
-      <c r="N41" s="98">
+      <c r="N41" s="37">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -4349,8 +4348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20AFEFDD-6C52-4CB7-9443-2E3596023181}">
   <dimension ref="A3:W54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4360,88 +4359,88 @@
   <sheetData>
     <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="97" t="s">
+      <c r="A4" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="96"/>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
-      <c r="G4" s="96"/>
-      <c r="H4" s="96"/>
-      <c r="I4" s="96"/>
-      <c r="J4" s="96"/>
-      <c r="K4" s="96"/>
-      <c r="L4" s="96"/>
-      <c r="M4" s="96"/>
-      <c r="N4" s="96"/>
-      <c r="O4" s="96"/>
-      <c r="P4" s="96"/>
-      <c r="Q4" s="96"/>
-      <c r="R4" s="96"/>
-      <c r="S4" s="96"/>
-      <c r="T4" s="96"/>
-      <c r="U4" s="96"/>
-      <c r="V4" s="96"/>
-      <c r="W4" s="95"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61"/>
+      <c r="M4" s="61"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="61"/>
+      <c r="P4" s="61"/>
+      <c r="Q4" s="61"/>
+      <c r="R4" s="61"/>
+      <c r="S4" s="61"/>
+      <c r="T4" s="61"/>
+      <c r="U4" s="61"/>
+      <c r="V4" s="61"/>
+      <c r="W4" s="62"/>
     </row>
     <row r="5" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="94"/>
-      <c r="B5" s="93"/>
-      <c r="C5" s="93"/>
-      <c r="D5" s="93"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="93"/>
-      <c r="H5" s="93"/>
-      <c r="I5" s="93"/>
-      <c r="J5" s="93"/>
-      <c r="K5" s="93"/>
-      <c r="L5" s="93"/>
-      <c r="M5" s="93"/>
-      <c r="N5" s="93"/>
-      <c r="O5" s="93"/>
-      <c r="P5" s="93"/>
-      <c r="Q5" s="93"/>
-      <c r="R5" s="93"/>
-      <c r="S5" s="93"/>
-      <c r="T5" s="93"/>
-      <c r="U5" s="93"/>
-      <c r="V5" s="93"/>
-      <c r="W5" s="92"/>
+      <c r="A5" s="63"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="64"/>
+      <c r="J5" s="64"/>
+      <c r="K5" s="64"/>
+      <c r="L5" s="64"/>
+      <c r="M5" s="64"/>
+      <c r="N5" s="64"/>
+      <c r="O5" s="64"/>
+      <c r="P5" s="64"/>
+      <c r="Q5" s="64"/>
+      <c r="R5" s="64"/>
+      <c r="S5" s="64"/>
+      <c r="T5" s="64"/>
+      <c r="U5" s="64"/>
+      <c r="V5" s="64"/>
+      <c r="W5" s="65"/>
     </row>
     <row r="6" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" s="50" t="s">
+      <c r="A7" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="B7" s="49"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="47" t="s">
+      <c r="B7" s="55"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="45"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="53"/>
       <c r="H7" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="63" t="s">
+      <c r="A8" s="57"/>
+      <c r="B8" s="58"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="E8" s="62" t="s">
+      <c r="E8" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="62" t="s">
+      <c r="F8" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="G8" s="39" t="s">
+      <c r="G8" s="23" t="s">
         <v>70</v>
       </c>
       <c r="H8" t="s">
@@ -4449,308 +4448,308 @@
       </c>
     </row>
     <row r="9" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="27">
+      <c r="C9" s="20">
         <f>D9*POWER(1+E9,F9)</f>
         <v>1628.8946267774415</v>
       </c>
-      <c r="D9" s="57">
+      <c r="D9" s="26">
         <v>1000</v>
       </c>
-      <c r="E9" s="91">
+      <c r="E9" s="36">
         <v>0.05</v>
       </c>
-      <c r="F9" s="56">
+      <c r="F9" s="25">
         <v>10</v>
       </c>
-      <c r="G9" s="90">
+      <c r="G9" s="35">
         <f>C9</f>
         <v>1628.8946267774415</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
-      <c r="B10" s="28" t="s">
+      <c r="A10" s="48"/>
+      <c r="B10" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="27">
+      <c r="C10" s="20">
         <f>-FV(E9,F9,,D9)</f>
         <v>1628.8946267774415</v>
       </c>
-      <c r="D10" s="89"/>
+      <c r="D10" s="34"/>
       <c r="E10" s="1"/>
-      <c r="G10" s="89"/>
+      <c r="G10" s="34"/>
     </row>
     <row r="11" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="88" t="s">
+      <c r="A11" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="27">
+      <c r="C11" s="20">
         <f>-PV(E9,F9,,G9)</f>
         <v>1000</v>
       </c>
     </row>
     <row r="12" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="87"/>
-      <c r="B12" s="25" t="s">
+      <c r="A12" s="50"/>
+      <c r="B12" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="24">
+      <c r="C12" s="18">
         <f>G9/POWER(1+E9,F9)</f>
         <v>1000</v>
       </c>
     </row>
     <row r="14" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15" s="50" t="s">
+      <c r="A15" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="49"/>
-      <c r="C15" s="86" t="s">
+      <c r="B15" s="55"/>
+      <c r="C15" s="70" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="86"/>
-      <c r="E15" s="86"/>
-      <c r="F15" s="86"/>
-      <c r="G15" s="86"/>
-      <c r="H15" s="85"/>
+      <c r="D15" s="70"/>
+      <c r="E15" s="70"/>
+      <c r="F15" s="70"/>
+      <c r="G15" s="70"/>
+      <c r="H15" s="71"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16" s="44"/>
-      <c r="B16" s="43"/>
-      <c r="C16" s="84" t="s">
+      <c r="A16" s="57"/>
+      <c r="B16" s="58"/>
+      <c r="C16" s="69" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="84"/>
-      <c r="E16" s="84" t="s">
+      <c r="D16" s="69"/>
+      <c r="E16" s="69" t="s">
         <v>65</v>
       </c>
-      <c r="F16" s="84"/>
-      <c r="G16" s="84" t="s">
+      <c r="F16" s="69"/>
+      <c r="G16" s="69" t="s">
         <v>64</v>
       </c>
-      <c r="H16" s="83"/>
+      <c r="H16" s="72"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="82">
-        <f>POWER(1+(C17/F17),H17) -1</f>
-        <v>0.14999999999999991</v>
-      </c>
-      <c r="B17" s="81"/>
-      <c r="C17" s="80">
-        <v>0.15</v>
-      </c>
-      <c r="D17" s="80"/>
-      <c r="E17" s="28" t="s">
+      <c r="A17" s="66">
+        <f t="shared" ref="A17:A32" si="0">POWER(1+(C17/F17),H17) -1</f>
+        <v>0.12000000000000011</v>
+      </c>
+      <c r="B17" s="67"/>
+      <c r="C17" s="68">
+        <v>0.12</v>
+      </c>
+      <c r="D17" s="68"/>
+      <c r="E17" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="F17" s="28">
+      <c r="F17" s="21">
         <v>1</v>
       </c>
-      <c r="G17" s="79" t="s">
+      <c r="G17" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="H17" s="78">
+      <c r="H17" s="32">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="82">
-        <f>POWER(1+(C18/F18),H18) -1</f>
+      <c r="A18" s="66">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B18" s="81"/>
-      <c r="C18" s="80">
-        <f>C17</f>
-        <v>0.15</v>
-      </c>
-      <c r="D18" s="80"/>
-      <c r="E18" s="28" t="s">
+      <c r="B18" s="67"/>
+      <c r="C18" s="68">
+        <f t="shared" ref="C18:C32" si="1">C17</f>
+        <v>0.12</v>
+      </c>
+      <c r="D18" s="68"/>
+      <c r="E18" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="F18" s="28">
+      <c r="F18" s="21">
         <v>1</v>
       </c>
-      <c r="G18" s="79" t="s">
+      <c r="G18" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="H18" s="78">
+      <c r="H18" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="82">
-        <f>POWER(1+(C19/F19),H19) -1</f>
+      <c r="A19" s="66">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B19" s="81"/>
-      <c r="C19" s="80">
-        <f>C18</f>
-        <v>0.15</v>
-      </c>
-      <c r="D19" s="80"/>
-      <c r="E19" s="28" t="s">
+      <c r="B19" s="67"/>
+      <c r="C19" s="68">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="D19" s="68"/>
+      <c r="E19" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="F19" s="28">
+      <c r="F19" s="21">
         <v>1</v>
       </c>
-      <c r="G19" s="79" t="s">
+      <c r="G19" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="H19" s="78">
+      <c r="H19" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="82">
-        <f>POWER(1+(C20/F20),H20) -1</f>
+      <c r="A20" s="66">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B20" s="81"/>
-      <c r="C20" s="80">
-        <f>C19</f>
-        <v>0.15</v>
-      </c>
-      <c r="D20" s="80"/>
-      <c r="E20" s="28" t="s">
+      <c r="B20" s="67"/>
+      <c r="C20" s="68">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="D20" s="68"/>
+      <c r="E20" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="F20" s="28">
+      <c r="F20" s="21">
         <v>1</v>
       </c>
-      <c r="G20" s="79" t="s">
+      <c r="G20" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="H20" s="78">
+      <c r="H20" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="82">
+      <c r="A21" s="66">
         <f>POWER(1+(C21/F21),H21) -1</f>
-        <v>0.1556249999999999</v>
-      </c>
-      <c r="B21" s="81"/>
-      <c r="C21" s="80">
-        <f>C20</f>
-        <v>0.15</v>
-      </c>
-      <c r="D21" s="80"/>
-      <c r="E21" s="28" t="s">
+        <v>0.12360000000000015</v>
+      </c>
+      <c r="B21" s="67"/>
+      <c r="C21" s="68">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="D21" s="68"/>
+      <c r="E21" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="F21" s="28">
+      <c r="F21" s="21">
         <v>2</v>
       </c>
-      <c r="G21" s="79" t="s">
+      <c r="G21" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="H21" s="78">
+      <c r="H21" s="32">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="82">
-        <f>POWER(1+(C22/F22),H22) -1</f>
-        <v>7.4999999999999956E-2</v>
-      </c>
-      <c r="B22" s="81"/>
-      <c r="C22" s="80">
-        <f>C21</f>
-        <v>0.15</v>
-      </c>
-      <c r="D22" s="80"/>
-      <c r="E22" s="28" t="s">
+      <c r="A22" s="66">
+        <f t="shared" si="0"/>
+        <v>6.0000000000000053E-2</v>
+      </c>
+      <c r="B22" s="67"/>
+      <c r="C22" s="68">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="D22" s="68"/>
+      <c r="E22" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="F22" s="28">
+      <c r="F22" s="21">
         <v>2</v>
       </c>
-      <c r="G22" s="79" t="s">
+      <c r="G22" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="H22" s="78">
+      <c r="H22" s="32">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="82">
-        <f>POWER(1+(C23/F23),H23) -1</f>
+      <c r="A23" s="66">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B23" s="81"/>
-      <c r="C23" s="80">
-        <f>C22</f>
-        <v>0.15</v>
-      </c>
-      <c r="D23" s="80"/>
-      <c r="E23" s="28" t="s">
+      <c r="B23" s="67"/>
+      <c r="C23" s="68">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="D23" s="68"/>
+      <c r="E23" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="F23" s="28">
+      <c r="F23" s="21">
         <v>2</v>
       </c>
-      <c r="G23" s="79" t="s">
+      <c r="G23" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="H23" s="78">
+      <c r="H23" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="82">
-        <f>POWER(1+(C24/F24),H24) -1</f>
+      <c r="A24" s="66">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B24" s="81"/>
-      <c r="C24" s="80">
-        <f>C23</f>
-        <v>0.15</v>
-      </c>
-      <c r="D24" s="80"/>
-      <c r="E24" s="28" t="s">
+      <c r="B24" s="67"/>
+      <c r="C24" s="68">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="D24" s="68"/>
+      <c r="E24" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="F24" s="28">
+      <c r="F24" s="21">
         <v>2</v>
       </c>
-      <c r="G24" s="79" t="s">
+      <c r="G24" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="H24" s="78">
+      <c r="H24" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="82">
-        <f>POWER(1+(C25/F25),H25) -1</f>
-        <v>0.15865041503906308</v>
-      </c>
-      <c r="B25" s="81"/>
-      <c r="C25" s="80">
-        <f>C24</f>
-        <v>0.15</v>
-      </c>
-      <c r="D25" s="80"/>
-      <c r="E25" s="28" t="s">
+      <c r="A25" s="66">
+        <f t="shared" si="0"/>
+        <v>0.12550880999999992</v>
+      </c>
+      <c r="B25" s="67"/>
+      <c r="C25" s="68">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="D25" s="68"/>
+      <c r="E25" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="F25" s="28">
+      <c r="F25" s="21">
         <v>4</v>
       </c>
-      <c r="G25" s="79" t="s">
+      <c r="G25" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="H25" s="78">
+      <c r="H25" s="32">
         <v>4</v>
       </c>
       <c r="L25" t="s">
@@ -4758,342 +4757,342 @@
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="82">
-        <f>POWER(1+(C26/F26),H26) -1</f>
-        <v>7.6406250000000231E-2</v>
-      </c>
-      <c r="B26" s="81"/>
-      <c r="C26" s="80">
-        <f>C25</f>
-        <v>0.15</v>
-      </c>
-      <c r="D26" s="80"/>
-      <c r="E26" s="28" t="s">
+      <c r="A26" s="66">
+        <f t="shared" si="0"/>
+        <v>6.0899999999999954E-2</v>
+      </c>
+      <c r="B26" s="67"/>
+      <c r="C26" s="68">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="D26" s="68"/>
+      <c r="E26" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="F26" s="28">
+      <c r="F26" s="21">
         <v>4</v>
       </c>
-      <c r="G26" s="79" t="s">
+      <c r="G26" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="H26" s="78">
+      <c r="H26" s="32">
         <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="82">
-        <f>POWER(1+(C27/F27),H27) -1</f>
-        <v>3.7500000000000089E-2</v>
-      </c>
-      <c r="B27" s="81"/>
-      <c r="C27" s="80">
-        <f>C26</f>
-        <v>0.15</v>
-      </c>
-      <c r="D27" s="80"/>
-      <c r="E27" s="28" t="s">
+      <c r="A27" s="66">
+        <f t="shared" si="0"/>
+        <v>3.0000000000000027E-2</v>
+      </c>
+      <c r="B27" s="67"/>
+      <c r="C27" s="68">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="D27" s="68"/>
+      <c r="E27" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="F27" s="28">
+      <c r="F27" s="21">
         <v>4</v>
       </c>
-      <c r="G27" s="79" t="s">
+      <c r="G27" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="H27" s="78">
+      <c r="H27" s="32">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="82">
-        <f>POWER(1+(C28/F28),H28) -1</f>
+      <c r="A28" s="66">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B28" s="81"/>
-      <c r="C28" s="80">
-        <f>C27</f>
-        <v>0.15</v>
-      </c>
-      <c r="D28" s="80"/>
-      <c r="E28" s="28" t="s">
+      <c r="B28" s="67"/>
+      <c r="C28" s="68">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="D28" s="68"/>
+      <c r="E28" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="F28" s="28">
+      <c r="F28" s="21">
         <v>4</v>
       </c>
-      <c r="G28" s="79" t="s">
+      <c r="G28" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="H28" s="78">
+      <c r="H28" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="82">
-        <f>POWER(1+(C29/F29),H29) -1</f>
-        <v>0.16075451772299854</v>
-      </c>
-      <c r="B29" s="81"/>
-      <c r="C29" s="80">
-        <f>C28</f>
-        <v>0.15</v>
-      </c>
-      <c r="D29" s="80"/>
-      <c r="E29" s="28" t="s">
+      <c r="A29" s="66">
+        <f t="shared" si="0"/>
+        <v>0.12682503013196977</v>
+      </c>
+      <c r="B29" s="67"/>
+      <c r="C29" s="68">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="D29" s="68"/>
+      <c r="E29" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="F29" s="28">
+      <c r="F29" s="21">
         <v>12</v>
       </c>
-      <c r="G29" s="79" t="s">
+      <c r="G29" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="H29" s="78">
+      <c r="H29" s="32">
         <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="82">
-        <f>POWER(1+(C30/F30),H30) -1</f>
-        <v>7.7383180545806729E-2</v>
-      </c>
-      <c r="B30" s="81"/>
-      <c r="C30" s="80">
-        <f>C29</f>
-        <v>0.15</v>
-      </c>
-      <c r="D30" s="80"/>
-      <c r="E30" s="28" t="s">
+      <c r="A30" s="66">
+        <f t="shared" si="0"/>
+        <v>6.1520150601000134E-2</v>
+      </c>
+      <c r="B30" s="67"/>
+      <c r="C30" s="68">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="D30" s="68"/>
+      <c r="E30" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="F30" s="28">
+      <c r="F30" s="21">
         <v>12</v>
       </c>
-      <c r="G30" s="79" t="s">
+      <c r="G30" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="H30" s="78">
+      <c r="H30" s="32">
         <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="82">
-        <f>POWER(1+(C31/F31),H31) -1</f>
-        <v>3.7970703124999838E-2</v>
-      </c>
-      <c r="B31" s="81"/>
-      <c r="C31" s="80">
-        <f>C30</f>
-        <v>0.15</v>
-      </c>
-      <c r="D31" s="80"/>
-      <c r="E31" s="28" t="s">
+      <c r="A31" s="66">
+        <f t="shared" si="0"/>
+        <v>3.0300999999999911E-2</v>
+      </c>
+      <c r="B31" s="67"/>
+      <c r="C31" s="68">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="D31" s="68"/>
+      <c r="E31" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="F31" s="28">
+      <c r="F31" s="21">
         <v>12</v>
       </c>
-      <c r="G31" s="79" t="s">
+      <c r="G31" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="H31" s="78">
+      <c r="H31" s="32">
         <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="77">
-        <f>POWER(1+(C32/F32),H32) -1</f>
-        <v>1.2499999999999956E-2</v>
-      </c>
-      <c r="B32" s="76"/>
+      <c r="A32" s="79">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000009E-2</v>
+      </c>
+      <c r="B32" s="80"/>
       <c r="C32" s="75">
-        <f>C31</f>
-        <v>0.15</v>
+        <f t="shared" si="1"/>
+        <v>0.12</v>
       </c>
       <c r="D32" s="75"/>
-      <c r="E32" s="25" t="s">
+      <c r="E32" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="F32" s="25">
+      <c r="F32" s="19">
         <v>12</v>
       </c>
-      <c r="G32" s="74" t="s">
+      <c r="G32" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="H32" s="73">
+      <c r="H32" s="30">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="50" t="s">
+      <c r="A38" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="B38" s="49"/>
-      <c r="C38" s="48"/>
-      <c r="D38" s="72" t="s">
+      <c r="B38" s="55"/>
+      <c r="C38" s="56"/>
+      <c r="D38" s="76" t="s">
         <v>49</v>
       </c>
-      <c r="E38" s="68"/>
-      <c r="F38" s="68"/>
-      <c r="G38" s="67"/>
+      <c r="E38" s="77"/>
+      <c r="F38" s="77"/>
+      <c r="G38" s="78"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="44"/>
-      <c r="B39" s="43"/>
-      <c r="C39" s="42"/>
-      <c r="D39" s="63" t="s">
+      <c r="A39" s="57"/>
+      <c r="B39" s="58"/>
+      <c r="C39" s="59"/>
+      <c r="D39" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="E39" s="62" t="s">
+      <c r="E39" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F39" s="40" t="s">
+      <c r="F39" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="G39" s="61"/>
+      <c r="G39" s="84"/>
     </row>
     <row r="40" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="60" t="s">
+      <c r="A40" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B40" s="59">
+      <c r="B40" s="81">
         <f>-PMT(F40,E40,D40)</f>
         <v>11379731.896831043</v>
       </c>
-      <c r="C40" s="58"/>
-      <c r="D40" s="57">
+      <c r="C40" s="82"/>
+      <c r="D40" s="26">
         <v>65000000</v>
       </c>
-      <c r="E40" s="56">
+      <c r="E40" s="25">
         <v>8</v>
       </c>
-      <c r="F40" s="55">
+      <c r="F40" s="85">
         <v>8.1600000000000006E-2</v>
       </c>
-      <c r="G40" s="54"/>
+      <c r="G40" s="86"/>
     </row>
     <row r="41" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="53" t="s">
+      <c r="A41" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="B41" s="52">
+      <c r="B41" s="73">
         <f>D40*(F40*POWER(1+F40,E40)/(POWER(1+F40,E40)-1))</f>
         <v>11379731.896831054</v>
       </c>
-      <c r="C41" s="51"/>
+      <c r="C41" s="74"/>
     </row>
     <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="71" t="s">
+      <c r="A43" s="93" t="s">
         <v>52</v>
       </c>
-      <c r="B43" s="70"/>
-      <c r="C43" s="69"/>
-      <c r="D43" s="68" t="s">
+      <c r="B43" s="94"/>
+      <c r="C43" s="95"/>
+      <c r="D43" s="77" t="s">
         <v>49</v>
       </c>
-      <c r="E43" s="68"/>
-      <c r="F43" s="68"/>
-      <c r="G43" s="67"/>
+      <c r="E43" s="77"/>
+      <c r="F43" s="77"/>
+      <c r="G43" s="78"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="66"/>
-      <c r="B44" s="65"/>
-      <c r="C44" s="64"/>
-      <c r="D44" s="63" t="s">
+      <c r="A44" s="96"/>
+      <c r="B44" s="97"/>
+      <c r="C44" s="98"/>
+      <c r="D44" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="E44" s="62" t="s">
+      <c r="E44" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F44" s="40" t="s">
+      <c r="F44" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="G44" s="61"/>
+      <c r="G44" s="84"/>
     </row>
     <row r="45" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="60" t="s">
+      <c r="A45" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B45" s="59">
+      <c r="B45" s="81">
         <f>-PV(F45,E45,D45)</f>
         <v>294.03131444078036</v>
       </c>
-      <c r="C45" s="58"/>
-      <c r="D45" s="57">
+      <c r="C45" s="82"/>
+      <c r="D45" s="26">
         <v>110</v>
       </c>
-      <c r="E45" s="56">
+      <c r="E45" s="25">
         <v>3</v>
       </c>
-      <c r="F45" s="55">
+      <c r="F45" s="85">
         <v>0.06</v>
       </c>
-      <c r="G45" s="54"/>
+      <c r="G45" s="86"/>
     </row>
     <row r="46" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="53" t="s">
+      <c r="A46" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="B46" s="52">
+      <c r="B46" s="73">
         <f>D45*((POWER(1+F45,E45)-1)/(F45*POWER(1+F45,E45)))</f>
         <v>294.03131444078036</v>
       </c>
-      <c r="C46" s="51"/>
+      <c r="C46" s="74"/>
     </row>
     <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A49" s="50" t="s">
+      <c r="A49" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="B49" s="49"/>
-      <c r="C49" s="48"/>
-      <c r="D49" s="47" t="s">
+      <c r="B49" s="55"/>
+      <c r="C49" s="56"/>
+      <c r="D49" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="E49" s="46"/>
-      <c r="F49" s="46"/>
-      <c r="G49" s="46"/>
-      <c r="H49" s="45"/>
+      <c r="E49" s="52"/>
+      <c r="F49" s="52"/>
+      <c r="G49" s="52"/>
+      <c r="H49" s="53"/>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A50" s="44"/>
-      <c r="B50" s="43"/>
-      <c r="C50" s="42"/>
-      <c r="D50" s="41" t="s">
+      <c r="A50" s="57"/>
+      <c r="B50" s="58"/>
+      <c r="C50" s="59"/>
+      <c r="D50" s="99" t="s">
         <v>48</v>
       </c>
-      <c r="E50" s="40"/>
-      <c r="F50" s="40" t="s">
+      <c r="E50" s="83"/>
+      <c r="F50" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="G50" s="40"/>
-      <c r="H50" s="39" t="s">
+      <c r="G50" s="83"/>
+      <c r="H50" s="23" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="51" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="32" t="s">
+      <c r="A51" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="B51" s="38" t="s">
+      <c r="B51" s="89" t="s">
         <v>42</v>
       </c>
-      <c r="C51" s="37">
+      <c r="C51" s="91">
         <f>D51*F51*H51</f>
         <v>1357350.3</v>
       </c>
-      <c r="D51" s="36">
+      <c r="D51" s="102">
         <v>45245010</v>
       </c>
-      <c r="E51" s="34"/>
-      <c r="F51" s="35">
+      <c r="E51" s="101"/>
+      <c r="F51" s="100">
         <v>0.01</v>
       </c>
-      <c r="G51" s="34"/>
-      <c r="H51" s="33">
+      <c r="G51" s="101"/>
+      <c r="H51" s="22">
         <v>3</v>
       </c>
       <c r="O51" t="s">
@@ -5101,30 +5100,30 @@
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A52" s="32"/>
-      <c r="B52" s="31"/>
-      <c r="C52" s="30"/>
-      <c r="D52" s="20"/>
-      <c r="E52" s="20"/>
+      <c r="A52" s="48"/>
+      <c r="B52" s="90"/>
+      <c r="C52" s="92"/>
+      <c r="D52" s="47"/>
+      <c r="E52" s="47"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A53" s="29" t="s">
+      <c r="A53" s="87" t="s">
         <v>43</v>
       </c>
-      <c r="B53" s="28" t="s">
+      <c r="B53" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="C53" s="27">
+      <c r="C53" s="20">
         <f>D51*(POWER(1+F51,H51)-1)</f>
         <v>1370969.0480099961</v>
       </c>
     </row>
     <row r="54" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="26"/>
-      <c r="B54" s="25" t="s">
+      <c r="A54" s="88"/>
+      <c r="B54" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C54" s="24">
+      <c r="C54" s="18">
         <f>-FV(F51,H51,,D51)-D51</f>
         <v>1370969.0480099991</v>
       </c>
@@ -5134,13 +5133,6 @@
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="A49:C50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D52:E52"/>
     <mergeCell ref="A43:C44"/>
     <mergeCell ref="D43:G43"/>
     <mergeCell ref="F44:G44"/>
@@ -5151,17 +5143,19 @@
     <mergeCell ref="B51:B52"/>
     <mergeCell ref="C51:C52"/>
     <mergeCell ref="B46:C46"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="A49:C50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D52:E52"/>
     <mergeCell ref="D38:G38"/>
     <mergeCell ref="A31:B31"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="F39:G39"/>
     <mergeCell ref="F40:G40"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="A38:C39"/>
     <mergeCell ref="A21:B21"/>
@@ -5173,11 +5167,20 @@
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="C32:D32"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="A15:B16"/>
     <mergeCell ref="C15:H15"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C29:D29"/>
@@ -5186,8 +5189,6 @@
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="C27:D27"/>
@@ -5197,8 +5198,6 @@
     <mergeCell ref="D7:G7"/>
     <mergeCell ref="A7:C8"/>
     <mergeCell ref="A4:W5"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
vault backup: 2024-10-08 11:27:59
</commit_message>
<xml_diff>
--- a/2024-2/Evaluación de proyectos/Excels/Ejercicios_sol_1.xlsx
+++ b/2024-2/Evaluación de proyectos/Excels/Ejercicios_sol_1.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
-  <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IVAN\Desktop\Codes\Apuntes_2024\2024-2\Evaluación de proyectos\Excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivaaan\Desktop\git\Apuntes_2024\2024-2\Evaluación de proyectos\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FB8760-9455-421B-AEDB-1EE0D9119A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB929801-E18A-4197-9349-6237087D9F5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="990" windowWidth="26100" windowHeight="14100" activeTab="2" xr2:uid="{C81B0A03-BDB8-4836-9CA0-B318B652DAA5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{C81B0A03-BDB8-4836-9CA0-B318B652DAA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Ej Aprovación de credito" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="89">
   <si>
     <t>TASA REAL EFECTIVA CREDITO</t>
   </si>
@@ -131,9 +131,6 @@
     <t xml:space="preserve">Suma de VENTA UNIDS </t>
   </si>
   <si>
-    <t>Etiquetas de fila</t>
-  </si>
-  <si>
     <t>Total general</t>
   </si>
   <si>
@@ -312,6 +309,9 @@
   </si>
   <si>
     <t>TIR</t>
+  </si>
+  <si>
+    <t>Etiquetas de columna</t>
   </si>
 </sst>
 </file>
@@ -966,6 +966,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -983,18 +995,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1028,38 +1028,126 @@
       <c:style val="2"/>
     </mc:Fallback>
   </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[Ejercicios_sol_1.xlsx]Tabla dinámica!TablaDinámica1</c:name>
+    <c:fmtId val="3"/>
+  </c:pivotSource>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-CL"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CL"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CL"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -1068,6 +1156,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Tabla dinámica'!$H$3:$H$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PRODUCTO A</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -1080,91 +1179,157 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="exp"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="es-CL"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:cat>
             <c:strRef>
-              <c:f>'Tabla dinámica'!$C$4:$C$24</c:f>
+              <c:f>'Tabla dinámica'!$G$5:$G$15</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>PRODUCTO B</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>PRODUCTO B</c:v>
+                  <c:v>2001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>PRODUCTO B</c:v>
+                  <c:v>2002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>PRODUCTO B</c:v>
+                  <c:v>2003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>PRODUCTO B</c:v>
+                  <c:v>2004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>PRODUCTO B</c:v>
+                  <c:v>2005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>PRODUCTO B</c:v>
+                  <c:v>2006</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>PRODUCTO B</c:v>
+                  <c:v>2007</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>PRODUCTO B</c:v>
+                  <c:v>2008</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>PRODUCTO B</c:v>
+                  <c:v>2009</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Tabla dinámica'!$D$4:$D$24</c:f>
+              <c:f>'Tabla dinámica'!$H$5:$H$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>171</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>186</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E1E2-406C-83A4-36C388B3D68D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Tabla dinámica'!$I$3:$I$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PRODUCTO B</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Tabla dinámica'!$G$5:$G$15</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2009</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Tabla dinámica'!$I$5:$I$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1204,7 +1369,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-389C-461A-9067-2C08F0287A51}"/>
+              <c16:uniqueId val="{00000005-E1E2-406C-83A4-36C388B3D68D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1217,11 +1382,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1471512320"/>
-        <c:axId val="1471508480"/>
+        <c:axId val="1539835407"/>
+        <c:axId val="1539845967"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1471512320"/>
+        <c:axId val="1539835407"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1264,7 +1429,7 @@
             <a:endParaRPr lang="es-CL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1471508480"/>
+        <c:crossAx val="1539845967"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1272,7 +1437,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1471508480"/>
+        <c:axId val="1539845967"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1323,7 +1488,7 @@
             <a:endParaRPr lang="es-CL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1471512320"/>
+        <c:crossAx val="1539835407"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1335,6 +1500,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1376,6 +1572,22 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
 </c:chartSpace>
 </file>
 
@@ -1988,23 +2200,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>179070</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>655320</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>41910</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1">
+        <xdr:cNvPr id="3" name="Gráfico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A49DBE1B-FA44-3349-72AF-C2B4E132C8B1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91DD9AD7-26E3-5D6D-91AB-D75A78DD2802}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2397,11 +2609,25 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="IVAN" refreshedDate="45565.735745949074" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="21" xr:uid="{B98FC9E6-6D5E-4265-9919-719B74BFB05D}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Ivaaan" refreshedDate="45566.022896759256" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="20" xr:uid="{2B770BED-F5F0-4CCF-B0F3-32F378E65520}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="C3:D24" sheet="Tabla dinámica"/>
+    <worksheetSource ref="B3:D23" sheet="Tabla dinámica"/>
   </cacheSource>
-  <cacheFields count="2">
+  <cacheFields count="3">
+    <cacheField name="AÑO" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2000" maxValue="2009" count="10">
+        <n v="2000"/>
+        <n v="2001"/>
+        <n v="2002"/>
+        <n v="2003"/>
+        <n v="2004"/>
+        <n v="2005"/>
+        <n v="2006"/>
+        <n v="2007"/>
+        <n v="2008"/>
+        <n v="2009"/>
+      </sharedItems>
+    </cacheField>
     <cacheField name="PRODUCTO A" numFmtId="0">
       <sharedItems count="2">
         <s v="PRODUCTO A"/>
@@ -2421,99 +2647,130 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="21">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="20">
   <r>
+    <x v="0"/>
     <x v="0"/>
     <n v="100"/>
   </r>
   <r>
+    <x v="0"/>
     <x v="1"/>
     <n v="95"/>
   </r>
   <r>
+    <x v="1"/>
     <x v="0"/>
     <n v="117"/>
   </r>
   <r>
     <x v="1"/>
+    <x v="1"/>
     <n v="152"/>
   </r>
   <r>
+    <x v="2"/>
     <x v="0"/>
     <n v="120"/>
   </r>
   <r>
+    <x v="2"/>
     <x v="1"/>
     <n v="220"/>
   </r>
   <r>
+    <x v="3"/>
     <x v="0"/>
     <n v="139"/>
   </r>
   <r>
+    <x v="3"/>
     <x v="1"/>
     <n v="350"/>
   </r>
   <r>
+    <x v="4"/>
     <x v="0"/>
     <n v="158"/>
   </r>
   <r>
+    <x v="4"/>
     <x v="1"/>
     <n v="570"/>
   </r>
   <r>
+    <x v="5"/>
     <x v="0"/>
     <n v="165"/>
   </r>
   <r>
+    <x v="5"/>
     <x v="1"/>
     <n v="800"/>
   </r>
   <r>
+    <x v="6"/>
     <x v="0"/>
     <n v="171"/>
   </r>
   <r>
+    <x v="6"/>
     <x v="1"/>
     <n v="1300"/>
   </r>
   <r>
+    <x v="7"/>
     <x v="0"/>
     <n v="175"/>
   </r>
   <r>
+    <x v="7"/>
     <x v="1"/>
     <n v="1900"/>
   </r>
   <r>
+    <x v="8"/>
     <x v="0"/>
     <n v="180"/>
   </r>
   <r>
+    <x v="8"/>
     <x v="1"/>
     <n v="3000"/>
   </r>
   <r>
+    <x v="9"/>
     <x v="0"/>
     <n v="186"/>
   </r>
   <r>
+    <x v="9"/>
     <x v="1"/>
     <n v="4400"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <n v="198"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C56BEC62-8017-431D-B3BC-C82E605B6596}" name="TablaDinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="H4:I7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A825245F-B967-45B4-91E2-79856554F9A0}" name="TablaDinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" rowHeaderCaption="AÑO">
+  <location ref="G3:J15" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
+      <items count="11">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
       <items count="3">
         <item x="0"/>
         <item x="1"/>
@@ -2525,7 +2782,45 @@
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="3">
+  <rowItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="3">
     <i>
       <x/>
     </i>
@@ -2535,13 +2830,36 @@
     <i t="grand">
       <x/>
     </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="Suma de VENTA UNIDS " fld="1" baseField="0" baseItem="0"/>
+    <dataField name="Suma de VENTA UNIDS " fld="2" baseField="0" baseItem="0"/>
   </dataFields>
+  <chartFormats count="2">
+    <chartFormat chart="3" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -2877,16 +3195,16 @@
       <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="6:11" x14ac:dyDescent="0.3">
       <c r="G2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2894,7 +3212,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="3" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="6:11" x14ac:dyDescent="0.3">
       <c r="G3" s="2" t="s">
         <v>2</v>
       </c>
@@ -2902,7 +3220,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="6:11" x14ac:dyDescent="0.3">
       <c r="G4" s="2" t="s">
         <v>0</v>
       </c>
@@ -2911,7 +3229,7 @@
         <v>0.12682503013196977</v>
       </c>
     </row>
-    <row r="5" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="6:11" x14ac:dyDescent="0.3">
       <c r="G5" s="2" t="s">
         <v>4</v>
       </c>
@@ -2925,7 +3243,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="6:11" x14ac:dyDescent="0.3">
       <c r="G6" s="2" t="s">
         <v>3</v>
       </c>
@@ -2934,10 +3252,10 @@
         <v>2107535.6902545234</v>
       </c>
     </row>
-    <row r="7" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="6:11" x14ac:dyDescent="0.3">
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="6:11" x14ac:dyDescent="0.3">
       <c r="G8" s="2" t="s">
         <v>10</v>
       </c>
@@ -2947,7 +3265,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="6:11" x14ac:dyDescent="0.3">
       <c r="G9" s="2" t="s">
         <v>6</v>
       </c>
@@ -2962,7 +3280,7 @@
         <v>8500000</v>
       </c>
     </row>
-    <row r="10" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="6:11" x14ac:dyDescent="0.3">
       <c r="F10">
         <v>1</v>
       </c>
@@ -2983,7 +3301,7 @@
         <v>7470477.0658672191</v>
       </c>
     </row>
-    <row r="11" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="6:11" x14ac:dyDescent="0.3">
       <c r="F11">
         <v>2</v>
       </c>
@@ -3004,7 +3322,7 @@
         <v>6310384.8545914944</v>
       </c>
     </row>
-    <row r="12" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="6:11" x14ac:dyDescent="0.3">
       <c r="F12">
         <v>3</v>
       </c>
@@ -3025,7 +3343,7 @@
         <v>5003163.9136648625</v>
       </c>
     </row>
-    <row r="13" spans="6:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="13" spans="6:11" ht="21" x14ac:dyDescent="0.4">
       <c r="F13">
         <v>4</v>
       </c>
@@ -3050,7 +3368,7 @@
         <v>3883170.1012676763</v>
       </c>
     </row>
-    <row r="14" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="6:11" x14ac:dyDescent="0.3">
       <c r="F14">
         <v>5</v>
       </c>
@@ -3071,7 +3389,7 @@
         <v>1870330.9155350341</v>
       </c>
     </row>
-    <row r="15" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="6:11" x14ac:dyDescent="0.3">
       <c r="F15">
         <v>6</v>
       </c>
@@ -3092,7 +3410,7 @@
         <v>-3.9581209421157837E-9</v>
       </c>
     </row>
-    <row r="18" spans="7:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G18" s="42" t="s">
         <v>11</v>
       </c>
@@ -3100,7 +3418,7 @@
       <c r="I18" s="42"/>
       <c r="J18" s="42"/>
     </row>
-    <row r="19" spans="7:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G19" s="2" t="s">
         <v>12</v>
       </c>
@@ -3110,7 +3428,7 @@
       </c>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="7:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G20" s="6">
         <f>-FV(8%,3,,3650000)</f>
         <v>4597948.8000000007</v>
@@ -3122,20 +3440,20 @@
       </c>
       <c r="J20" s="2"/>
     </row>
-    <row r="22" spans="7:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G22" s="43" t="s">
         <v>14</v>
       </c>
       <c r="H22" s="44"/>
     </row>
-    <row r="23" spans="7:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G23" s="45">
         <f>K13-I20</f>
         <v>1584195.701267676</v>
       </c>
       <c r="H23" s="46"/>
     </row>
-    <row r="24" spans="7:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G24" s="2" t="s">
         <v>15</v>
       </c>
@@ -3143,7 +3461,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="25" spans="7:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G25" s="2" t="s">
         <v>16</v>
       </c>
@@ -3151,7 +3469,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="7:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G26" s="2" t="s">
         <v>3</v>
       </c>
@@ -3160,7 +3478,7 @@
         <v>614721.02489998355</v>
       </c>
     </row>
-    <row r="27" spans="7:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G27" s="2" t="s">
         <v>17</v>
       </c>
@@ -3170,7 +3488,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="7:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G28" s="2" t="s">
         <v>6</v>
       </c>
@@ -3185,7 +3503,7 @@
         <v>1584195.701267676</v>
       </c>
     </row>
-    <row r="29" spans="7:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G29" s="9">
         <f>$H$24*J28</f>
         <v>126735.65610141408</v>
@@ -3203,7 +3521,7 @@
         <v>1096210.3324691064</v>
       </c>
     </row>
-    <row r="30" spans="7:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G30" s="9">
         <f>$H$24*J29</f>
         <v>87696.826597528518</v>
@@ -3221,7 +3539,7 @@
         <v>569186.13416665141</v>
       </c>
     </row>
-    <row r="31" spans="7:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G31" s="9">
         <f>$H$24*J30</f>
         <v>45534.890733332111</v>
@@ -3239,12 +3557,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G33" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="7:9" x14ac:dyDescent="0.3">
       <c r="H34" t="s">
         <v>20</v>
       </c>
@@ -3252,7 +3570,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="35" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G35" s="2" t="s">
         <v>19</v>
       </c>
@@ -3263,7 +3581,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G36" s="2">
         <v>1</v>
       </c>
@@ -3275,7 +3593,7 @@
         <v>2046151.1555869158</v>
       </c>
     </row>
-    <row r="37" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G37" s="2">
         <v>2</v>
       </c>
@@ -3287,7 +3605,7 @@
         <v>1986554.519987297</v>
       </c>
     </row>
-    <row r="38" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G38" s="2">
         <v>3</v>
       </c>
@@ -3299,7 +3617,7 @@
         <v>1928693.7087255311</v>
       </c>
     </row>
-    <row r="39" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G39" s="2">
         <v>4</v>
       </c>
@@ -3311,7 +3629,7 @@
         <v>1872518.1638111954</v>
       </c>
     </row>
-    <row r="40" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G40" s="2">
         <v>5</v>
       </c>
@@ -3323,7 +3641,7 @@
         <v>530263.75602436229</v>
       </c>
     </row>
-    <row r="41" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G41" s="2">
         <v>6</v>
       </c>
@@ -3335,7 +3653,7 @@
         <v>514819.18060617696</v>
       </c>
     </row>
-    <row r="42" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G42" s="2">
         <v>7</v>
       </c>
@@ -3347,7 +3665,7 @@
         <v>499824.44719046302</v>
       </c>
     </row>
-    <row r="44" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G44" s="47" t="s">
         <v>22</v>
       </c>
@@ -3371,24 +3689,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5C1D520-EAF6-40A7-AC3A-61C23BF36621}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="B3:I24"/>
+  <dimension ref="B3:J24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+    <sheetView topLeftCell="A11" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="12" t="s">
         <v>23</v>
       </c>
@@ -3399,8 +3716,14 @@
         <v>25</v>
       </c>
       <c r="E3" s="12"/>
-    </row>
-    <row r="4" spans="2:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G3" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="12">
         <v>2000</v>
       </c>
@@ -3411,14 +3734,20 @@
         <v>100</v>
       </c>
       <c r="E4" s="12"/>
-      <c r="H4" s="13" t="s">
+      <c r="G4" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" t="s">
         <v>28</v>
       </c>
-      <c r="I4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="12">
         <v>2000</v>
       </c>
@@ -3429,14 +3758,20 @@
         <v>95</v>
       </c>
       <c r="E5" s="12"/>
-      <c r="H5" s="14" t="s">
-        <v>24</v>
+      <c r="G5" s="14">
+        <v>2000</v>
+      </c>
+      <c r="H5">
+        <v>100</v>
       </c>
       <c r="I5">
-        <v>1709</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="J5">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="12">
         <v>2001</v>
       </c>
@@ -3447,14 +3782,20 @@
         <v>117</v>
       </c>
       <c r="E6" s="12"/>
-      <c r="H6" s="14" t="s">
-        <v>26</v>
+      <c r="G6" s="14">
+        <v>2001</v>
+      </c>
+      <c r="H6">
+        <v>117</v>
       </c>
       <c r="I6">
-        <v>12787</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+      <c r="J6">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="12">
         <v>2001</v>
       </c>
@@ -3465,14 +3806,20 @@
         <v>152</v>
       </c>
       <c r="E7" s="12"/>
-      <c r="H7" s="14" t="s">
-        <v>29</v>
+      <c r="G7" s="14">
+        <v>2002</v>
+      </c>
+      <c r="H7">
+        <v>120</v>
       </c>
       <c r="I7">
-        <v>14496</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+      <c r="J7">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="12">
         <v>2002</v>
       </c>
@@ -3483,8 +3830,20 @@
         <v>120</v>
       </c>
       <c r="E8" s="12"/>
-    </row>
-    <row r="9" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G8" s="14">
+        <v>2003</v>
+      </c>
+      <c r="H8">
+        <v>139</v>
+      </c>
+      <c r="I8">
+        <v>350</v>
+      </c>
+      <c r="J8">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B9" s="12">
         <v>2002</v>
       </c>
@@ -3495,8 +3854,20 @@
         <v>220</v>
       </c>
       <c r="E9" s="12"/>
-    </row>
-    <row r="10" spans="2:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G9" s="14">
+        <v>2004</v>
+      </c>
+      <c r="H9">
+        <v>158</v>
+      </c>
+      <c r="I9">
+        <v>570</v>
+      </c>
+      <c r="J9">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B10" s="12">
         <v>2003</v>
       </c>
@@ -3507,8 +3878,20 @@
         <v>139</v>
       </c>
       <c r="E10" s="12"/>
-    </row>
-    <row r="11" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G10" s="14">
+        <v>2005</v>
+      </c>
+      <c r="H10">
+        <v>165</v>
+      </c>
+      <c r="I10">
+        <v>800</v>
+      </c>
+      <c r="J10">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B11" s="12">
         <v>2003</v>
       </c>
@@ -3519,8 +3902,20 @@
         <v>350</v>
       </c>
       <c r="E11" s="12"/>
-    </row>
-    <row r="12" spans="2:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G11" s="14">
+        <v>2006</v>
+      </c>
+      <c r="H11">
+        <v>171</v>
+      </c>
+      <c r="I11">
+        <v>1300</v>
+      </c>
+      <c r="J11">
+        <v>1471</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B12" s="12">
         <v>2004</v>
       </c>
@@ -3531,8 +3926,20 @@
         <v>158</v>
       </c>
       <c r="E12" s="12"/>
-    </row>
-    <row r="13" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G12" s="14">
+        <v>2007</v>
+      </c>
+      <c r="H12">
+        <v>175</v>
+      </c>
+      <c r="I12">
+        <v>1900</v>
+      </c>
+      <c r="J12">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B13" s="12">
         <v>2004</v>
       </c>
@@ -3543,8 +3950,20 @@
         <v>570</v>
       </c>
       <c r="E13" s="12"/>
-    </row>
-    <row r="14" spans="2:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G13" s="14">
+        <v>2008</v>
+      </c>
+      <c r="H13">
+        <v>180</v>
+      </c>
+      <c r="I13">
+        <v>3000</v>
+      </c>
+      <c r="J13">
+        <v>3180</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B14" s="12">
         <v>2005</v>
       </c>
@@ -3555,8 +3974,20 @@
         <v>165</v>
       </c>
       <c r="E14" s="12"/>
-    </row>
-    <row r="15" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G14" s="14">
+        <v>2009</v>
+      </c>
+      <c r="H14">
+        <v>186</v>
+      </c>
+      <c r="I14">
+        <v>4400</v>
+      </c>
+      <c r="J14">
+        <v>4586</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B15" s="12">
         <v>2005</v>
       </c>
@@ -3567,8 +3998,20 @@
         <v>800</v>
       </c>
       <c r="E15" s="12"/>
-    </row>
-    <row r="16" spans="2:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G15" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H15">
+        <v>1511</v>
+      </c>
+      <c r="I15">
+        <v>12787</v>
+      </c>
+      <c r="J15">
+        <v>14298</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B16" s="12">
         <v>2006</v>
       </c>
@@ -3580,7 +4023,7 @@
       </c>
       <c r="E16" s="12"/>
     </row>
-    <row r="17" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B17" s="12">
         <v>2006</v>
       </c>
@@ -3592,7 +4035,7 @@
       </c>
       <c r="E17" s="12"/>
     </row>
-    <row r="18" spans="2:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B18" s="12">
         <v>2007</v>
       </c>
@@ -3604,7 +4047,7 @@
       </c>
       <c r="E18" s="12"/>
     </row>
-    <row r="19" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B19" s="12">
         <v>2007</v>
       </c>
@@ -3616,7 +4059,7 @@
       </c>
       <c r="E19" s="12"/>
     </row>
-    <row r="20" spans="2:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B20" s="12">
         <v>2008</v>
       </c>
@@ -3628,7 +4071,7 @@
       </c>
       <c r="E20" s="12"/>
     </row>
-    <row r="21" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B21" s="12">
         <v>2008</v>
       </c>
@@ -3640,7 +4083,7 @@
       </c>
       <c r="E21" s="12"/>
     </row>
-    <row r="22" spans="2:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B22" s="12">
         <v>2009</v>
       </c>
@@ -3652,7 +4095,7 @@
       </c>
       <c r="E22" s="12"/>
     </row>
-    <row r="23" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B23" s="12">
         <v>2009</v>
       </c>
@@ -3664,7 +4107,7 @@
       </c>
       <c r="E23" s="12"/>
     </row>
-    <row r="24" spans="2:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B24" s="12">
         <v>2010</v>
       </c>
@@ -3677,13 +4120,7 @@
       <c r="E24" s="12"/>
     </row>
   </sheetData>
-  <autoFilter ref="B3:E24" xr:uid="{D5C1D520-EAF6-40A7-AC3A-61C23BF36621}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="PRODUCTO B"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="B3:E24" xr:uid="{D5C1D520-EAF6-40A7-AC3A-61C23BF36621}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
 </worksheet>
@@ -3693,20 +4130,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C8269A2-8272-4B58-BB60-2DE0A7F360FB}">
   <dimension ref="J3:Q41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="G11" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="10" width="11.42578125" style="15"/>
+    <col min="1" max="10" width="11.44140625" style="15"/>
     <col min="11" max="11" width="27" style="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" style="15"/>
-    <col min="13" max="13" width="14.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="11.42578125" style="15"/>
+    <col min="12" max="12" width="11.44140625" style="15"/>
+    <col min="13" max="13" width="14.5546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="11.44140625" style="15"/>
   </cols>
   <sheetData>
-    <row r="3" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="10:17" x14ac:dyDescent="0.3">
       <c r="M3" s="15">
         <v>1</v>
       </c>
@@ -3723,14 +4160,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="10:17" x14ac:dyDescent="0.3">
       <c r="K4" s="16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="10:17" x14ac:dyDescent="0.3">
+      <c r="K5" s="15" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="K5" s="15" t="s">
-        <v>31</v>
       </c>
       <c r="M5" s="15">
         <v>1500</v>
@@ -3752,9 +4189,9 @@
         <v>2194.6982400000006</v>
       </c>
     </row>
-    <row r="6" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="10:17" x14ac:dyDescent="0.3">
       <c r="K6" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M6" s="15">
         <v>8000</v>
@@ -3776,9 +4213,9 @@
         <v>8830.5031249999993</v>
       </c>
     </row>
-    <row r="7" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="10:17" x14ac:dyDescent="0.3">
       <c r="K7" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M7" s="15">
         <f>M6*M5</f>
@@ -3801,14 +4238,14 @@
         <v>19380289.666752003</v>
       </c>
     </row>
-    <row r="9" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="10:17" x14ac:dyDescent="0.3">
       <c r="K9" s="16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="10:17" x14ac:dyDescent="0.3">
+      <c r="K10" s="15" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="K10" s="15" t="s">
-        <v>34</v>
       </c>
       <c r="M10" s="15">
         <v>-9000000</v>
@@ -3830,12 +4267,12 @@
         <v>-10939556.25</v>
       </c>
     </row>
-    <row r="11" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="10:17" x14ac:dyDescent="0.3">
       <c r="J11" s="15">
         <v>-1000</v>
       </c>
       <c r="K11" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M11" s="15">
         <f>$J$11*M5*POWER(1.025,M3-1)</f>
@@ -3858,13 +4295,13 @@
         <v>-2422536.2083440004</v>
       </c>
     </row>
-    <row r="12" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="10:17" x14ac:dyDescent="0.3">
       <c r="J12" s="15">
         <f>-(2000000+1500000)/12</f>
         <v>-291666.66666666669</v>
       </c>
       <c r="K12" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M12" s="15">
         <f>$J$12</f>
@@ -3887,9 +4324,9 @@
         <v>-291666.66666666669</v>
       </c>
     </row>
-    <row r="13" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="10:17" x14ac:dyDescent="0.3">
       <c r="K13" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M13" s="15">
         <v>-866333.70281249797</v>
@@ -3907,9 +4344,9 @@
         <v>-238930.627730281</v>
       </c>
     </row>
-    <row r="14" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="10:17" x14ac:dyDescent="0.3">
       <c r="K14" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M14" s="15">
         <f>-300000</f>
@@ -3932,9 +4369,9 @@
         <v>-331143.8671875</v>
       </c>
     </row>
-    <row r="15" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="10:17" x14ac:dyDescent="0.3">
       <c r="K15" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M15" s="15">
         <f>SUM(M10:M14)</f>
@@ -3957,9 +4394,9 @@
         <v>-14223833.619928448</v>
       </c>
     </row>
-    <row r="16" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="10:17" x14ac:dyDescent="0.3">
       <c r="K16" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M16" s="15">
         <f>M7+M15</f>
@@ -3982,12 +4419,12 @@
         <v>5156456.0468235556</v>
       </c>
     </row>
-    <row r="17" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="10:17" x14ac:dyDescent="0.3">
       <c r="J17" s="17">
         <v>-0.25</v>
       </c>
       <c r="K17" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M17" s="15">
         <f>$J$17*M16</f>
@@ -4010,9 +4447,9 @@
         <v>-1289114.0117058889</v>
       </c>
     </row>
-    <row r="19" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="10:17" x14ac:dyDescent="0.3">
       <c r="K19" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M19" s="15">
         <f>M16+M17</f>
@@ -4035,9 +4472,9 @@
         <v>3867342.0351176667</v>
       </c>
     </row>
-    <row r="20" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="10:17" x14ac:dyDescent="0.3">
       <c r="K20" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M20" s="15">
         <f>-M12</f>
@@ -4060,9 +4497,9 @@
         <v>291666.66666666669</v>
       </c>
     </row>
-    <row r="21" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="10:17" x14ac:dyDescent="0.3">
       <c r="K21" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M21" s="15">
         <v>-613675.06985862798</v>
@@ -4080,14 +4517,14 @@
         <v>-1241078.1449408401</v>
       </c>
     </row>
-    <row r="22" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="10:17" x14ac:dyDescent="0.3">
       <c r="K22" s="16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="10:17" x14ac:dyDescent="0.3">
+      <c r="K23" s="15" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="23" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="K23" s="15" t="s">
-        <v>81</v>
       </c>
       <c r="L23" s="15">
         <v>-1000000</v>
@@ -4097,9 +4534,9 @@
         <v>700000</v>
       </c>
     </row>
-    <row r="24" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="10:17" x14ac:dyDescent="0.3">
       <c r="K24" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L24" s="15">
         <v>-1500000</v>
@@ -4109,9 +4546,9 @@
         <v>1050000</v>
       </c>
     </row>
-    <row r="25" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="10:17" x14ac:dyDescent="0.3">
       <c r="K25" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L25" s="15">
         <v>-2000000</v>
@@ -4121,17 +4558,17 @@
         <v>1400000</v>
       </c>
     </row>
-    <row r="26" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="10:17" x14ac:dyDescent="0.3">
       <c r="K26" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L26" s="15">
         <v>4500000</v>
       </c>
     </row>
-    <row r="27" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="10:17" x14ac:dyDescent="0.3">
       <c r="K27" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L27" s="15">
         <f>1.5*M11</f>
@@ -4142,9 +4579,9 @@
         <v>1912500</v>
       </c>
     </row>
-    <row r="28" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="10:17" x14ac:dyDescent="0.3">
       <c r="K28" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L28" s="15">
         <f>SUM(L23:L27)</f>
@@ -4171,34 +4608,34 @@
         <v>7980430.5568434931</v>
       </c>
     </row>
-    <row r="29" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="10:17" x14ac:dyDescent="0.3">
       <c r="K29" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L29" s="40">
         <f>2%+1.2*10%</f>
         <v>0.13999999999999999</v>
       </c>
     </row>
-    <row r="30" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="10:17" x14ac:dyDescent="0.3">
       <c r="K30" s="39" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L30" s="39">
         <f>NPV(L29,M28:Q28)+L28</f>
         <v>3283327.9442483895</v>
       </c>
     </row>
-    <row r="31" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="10:17" x14ac:dyDescent="0.3">
       <c r="K31" s="39" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L31" s="41">
         <f>IRR(L28:Q28)</f>
         <v>0.3770042029363736</v>
       </c>
     </row>
-    <row r="33" spans="11:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K33" s="37" t="s">
         <v>6</v>
       </c>
@@ -4207,13 +4644,13 @@
         <v>0.19251860062499948</v>
       </c>
       <c r="M33" s="37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N33" s="37">
         <v>4500000</v>
       </c>
     </row>
-    <row r="34" spans="11:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K34" s="37" t="s">
         <v>7</v>
       </c>
@@ -4224,7 +4661,7 @@
       <c r="M34" s="37"/>
       <c r="N34" s="37"/>
     </row>
-    <row r="35" spans="11:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K35" s="37"/>
       <c r="L35" s="37"/>
       <c r="M35" s="37"/>
@@ -4232,7 +4669,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="11:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K36" s="37" t="s">
         <v>6</v>
       </c>
@@ -4247,7 +4684,7 @@
         <v>4500000</v>
       </c>
     </row>
-    <row r="37" spans="11:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K37" s="37">
         <f>$L$33*N36</f>
         <v>866333.70281249762</v>
@@ -4265,7 +4702,7 @@
         <v>3886324.9301413726</v>
       </c>
     </row>
-    <row r="38" spans="11:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K38" s="37">
         <f>$L$33*N37</f>
         <v>748189.83712486597</v>
@@ -4283,7 +4720,7 @@
         <v>3154505.9945951132</v>
       </c>
     </row>
-    <row r="39" spans="11:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K39" s="37">
         <f>$L$33*N38</f>
         <v>607301.07974262338</v>
@@ -4301,7 +4738,7 @@
         <v>2281798.3016666113</v>
       </c>
     </row>
-    <row r="40" spans="11:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K40" s="37">
         <f>$L$33*N39</f>
         <v>439288.61594535643</v>
@@ -4319,7 +4756,7 @@
         <v>1241078.1449408426</v>
       </c>
     </row>
-    <row r="41" spans="11:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K41" s="37">
         <f>$L$33*N40</f>
         <v>238930.6277302813</v>
@@ -4352,15 +4789,15 @@
       <selection activeCell="C18" sqref="C18:D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="60" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B4" s="61"/>
       <c r="C4" s="61"/>
@@ -4385,7 +4822,7 @@
       <c r="V4" s="61"/>
       <c r="W4" s="62"/>
     </row>
-    <row r="5" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="63"/>
       <c r="B5" s="64"/>
       <c r="C5" s="64"/>
@@ -4410,49 +4847,49 @@
       <c r="V5" s="64"/>
       <c r="W5" s="65"/>
     </row>
-    <row r="6" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="54" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B7" s="55"/>
       <c r="C7" s="56"/>
       <c r="D7" s="51" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E7" s="52"/>
       <c r="F7" s="52"/>
       <c r="G7" s="53"/>
       <c r="H7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="57"/>
       <c r="B8" s="58"/>
       <c r="C8" s="59"/>
       <c r="D8" s="29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E8" s="28" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="48" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9" s="20">
         <f>D9*POWER(1+E9,F9)</f>
@@ -4472,10 +4909,10 @@
         <v>1628.8946267774415</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="48"/>
       <c r="B10" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" s="20">
         <f>-FV(E9,F9,,D9)</f>
@@ -4485,36 +4922,36 @@
       <c r="E10" s="1"/>
       <c r="G10" s="34"/>
     </row>
-    <row r="11" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="49" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" s="20">
         <f>-PV(E9,F9,,G9)</f>
         <v>1000</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="50"/>
       <c r="B12" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C12" s="18">
         <f>G9/POWER(1+E9,F9)</f>
         <v>1000</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" s="54" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B15" s="55"/>
       <c r="C15" s="70" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D15" s="70"/>
       <c r="E15" s="70"/>
@@ -4522,23 +4959,23 @@
       <c r="G15" s="70"/>
       <c r="H15" s="71"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" s="57"/>
       <c r="B16" s="58"/>
       <c r="C16" s="69" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D16" s="69"/>
       <c r="E16" s="69" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F16" s="69"/>
       <c r="G16" s="69" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H16" s="72"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="66">
         <f t="shared" ref="A17:A32" si="0">POWER(1+(C17/F17),H17) -1</f>
         <v>0.12000000000000011</v>
@@ -4549,19 +4986,19 @@
       </c>
       <c r="D17" s="68"/>
       <c r="E17" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F17" s="21">
         <v>1</v>
       </c>
       <c r="G17" s="33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H17" s="32">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="66">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4573,19 +5010,19 @@
       </c>
       <c r="D18" s="68"/>
       <c r="E18" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F18" s="21">
         <v>1</v>
       </c>
       <c r="G18" s="33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H18" s="32">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="66">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4597,19 +5034,19 @@
       </c>
       <c r="D19" s="68"/>
       <c r="E19" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F19" s="21">
         <v>1</v>
       </c>
       <c r="G19" s="33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H19" s="32">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="66">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4621,19 +5058,19 @@
       </c>
       <c r="D20" s="68"/>
       <c r="E20" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F20" s="21">
         <v>1</v>
       </c>
       <c r="G20" s="33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H20" s="32">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="66">
         <f>POWER(1+(C21/F21),H21) -1</f>
         <v>0.12360000000000015</v>
@@ -4645,19 +5082,19 @@
       </c>
       <c r="D21" s="68"/>
       <c r="E21" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F21" s="21">
         <v>2</v>
       </c>
       <c r="G21" s="33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H21" s="32">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="66">
         <f t="shared" si="0"/>
         <v>6.0000000000000053E-2</v>
@@ -4669,19 +5106,19 @@
       </c>
       <c r="D22" s="68"/>
       <c r="E22" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F22" s="21">
         <v>2</v>
       </c>
       <c r="G22" s="33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H22" s="32">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="66">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4693,19 +5130,19 @@
       </c>
       <c r="D23" s="68"/>
       <c r="E23" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F23" s="21">
         <v>2</v>
       </c>
       <c r="G23" s="33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H23" s="32">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="66">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4717,19 +5154,19 @@
       </c>
       <c r="D24" s="68"/>
       <c r="E24" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F24" s="21">
         <v>2</v>
       </c>
       <c r="G24" s="33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H24" s="32">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="66">
         <f t="shared" si="0"/>
         <v>0.12550880999999992</v>
@@ -4741,22 +5178,22 @@
       </c>
       <c r="D25" s="68"/>
       <c r="E25" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F25" s="21">
         <v>4</v>
       </c>
       <c r="G25" s="33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H25" s="32">
         <v>4</v>
       </c>
       <c r="L25" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="66">
         <f t="shared" si="0"/>
         <v>6.0899999999999954E-2</v>
@@ -4768,19 +5205,19 @@
       </c>
       <c r="D26" s="68"/>
       <c r="E26" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F26" s="21">
         <v>4</v>
       </c>
       <c r="G26" s="33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H26" s="32">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="66">
         <f t="shared" si="0"/>
         <v>3.0000000000000027E-2</v>
@@ -4792,19 +5229,19 @@
       </c>
       <c r="D27" s="68"/>
       <c r="E27" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F27" s="21">
         <v>4</v>
       </c>
       <c r="G27" s="33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H27" s="32">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="66">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4816,19 +5253,19 @@
       </c>
       <c r="D28" s="68"/>
       <c r="E28" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F28" s="21">
         <v>4</v>
       </c>
       <c r="G28" s="33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H28" s="32">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="66">
         <f t="shared" si="0"/>
         <v>0.12682503013196977</v>
@@ -4840,19 +5277,19 @@
       </c>
       <c r="D29" s="68"/>
       <c r="E29" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F29" s="21">
         <v>12</v>
       </c>
       <c r="G29" s="33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H29" s="32">
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="66">
         <f t="shared" si="0"/>
         <v>6.1520150601000134E-2</v>
@@ -4864,19 +5301,19 @@
       </c>
       <c r="D30" s="68"/>
       <c r="E30" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F30" s="21">
         <v>12</v>
       </c>
       <c r="G30" s="33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H30" s="32">
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="66">
         <f t="shared" si="0"/>
         <v>3.0300999999999911E-2</v>
@@ -4888,19 +5325,19 @@
       </c>
       <c r="D31" s="68"/>
       <c r="E31" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F31" s="21">
         <v>12</v>
       </c>
       <c r="G31" s="33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H31" s="32">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="79">
         <f t="shared" si="0"/>
         <v>1.0000000000000009E-2</v>
@@ -4912,50 +5349,50 @@
       </c>
       <c r="D32" s="75"/>
       <c r="E32" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F32" s="19">
         <v>12</v>
       </c>
       <c r="G32" s="31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H32" s="30">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="54" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B38" s="55"/>
       <c r="C38" s="56"/>
       <c r="D38" s="76" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E38" s="77"/>
       <c r="F38" s="77"/>
       <c r="G38" s="78"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="57"/>
       <c r="B39" s="58"/>
       <c r="C39" s="59"/>
       <c r="D39" s="29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E39" s="28" t="s">
         <v>19</v>
       </c>
       <c r="F39" s="83" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G39" s="84"/>
     </row>
-    <row r="40" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B40" s="81">
         <f>-PMT(F40,E40,D40)</f>
@@ -4973,9 +5410,9 @@
       </c>
       <c r="G40" s="86"/>
     </row>
-    <row r="41" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B41" s="73">
         <f>D40*(F40*POWER(1+F40,E40)/(POWER(1+F40,E40)-1))</f>
@@ -4983,24 +5420,24 @@
       </c>
       <c r="C41" s="74"/>
     </row>
-    <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="93" t="s">
-        <v>52</v>
-      </c>
-      <c r="B43" s="94"/>
-      <c r="C43" s="95"/>
+    <row r="42" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" s="97" t="s">
+        <v>51</v>
+      </c>
+      <c r="B43" s="98"/>
+      <c r="C43" s="99"/>
       <c r="D43" s="77" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E43" s="77"/>
       <c r="F43" s="77"/>
       <c r="G43" s="78"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="96"/>
-      <c r="B44" s="97"/>
-      <c r="C44" s="98"/>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" s="100"/>
+      <c r="B44" s="101"/>
+      <c r="C44" s="102"/>
       <c r="D44" s="29" t="s">
         <v>7</v>
       </c>
@@ -5008,13 +5445,13 @@
         <v>19</v>
       </c>
       <c r="F44" s="83" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G44" s="84"/>
     </row>
-    <row r="45" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B45" s="81">
         <f>-PV(F45,E45,D45)</f>
@@ -5032,9 +5469,9 @@
       </c>
       <c r="G45" s="86"/>
     </row>
-    <row r="46" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B46" s="73">
         <f>D45*((POWER(1+F45,E45)-1)/(F45*POWER(1+F45,E45)))</f>
@@ -5042,93 +5479,93 @@
       </c>
       <c r="C46" s="74"/>
     </row>
-    <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B49" s="55"/>
       <c r="C49" s="56"/>
       <c r="D49" s="51" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E49" s="52"/>
       <c r="F49" s="52"/>
       <c r="G49" s="52"/>
       <c r="H49" s="53"/>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" s="57"/>
       <c r="B50" s="58"/>
       <c r="C50" s="59"/>
-      <c r="D50" s="99" t="s">
-        <v>48</v>
+      <c r="D50" s="93" t="s">
+        <v>47</v>
       </c>
       <c r="E50" s="83"/>
       <c r="F50" s="83" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G50" s="83"/>
       <c r="H50" s="23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="48" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B51" s="89" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C51" s="91">
         <f>D51*F51*H51</f>
         <v>1357350.3</v>
       </c>
-      <c r="D51" s="102">
+      <c r="D51" s="96">
         <v>45245010</v>
       </c>
-      <c r="E51" s="101"/>
-      <c r="F51" s="100">
+      <c r="E51" s="95"/>
+      <c r="F51" s="94">
         <v>0.01</v>
       </c>
-      <c r="G51" s="101"/>
+      <c r="G51" s="95"/>
       <c r="H51" s="22">
         <v>3</v>
       </c>
       <c r="O51" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" s="48"/>
       <c r="B52" s="90"/>
       <c r="C52" s="92"/>
       <c r="D52" s="47"/>
       <c r="E52" s="47"/>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" s="87" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B53" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C53" s="20">
         <f>D51*(POWER(1+F51,H51)-1)</f>
         <v>1370969.0480099961</v>
       </c>
     </row>
-    <row r="54" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="88"/>
       <c r="B54" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C54" s="18">
         <f>-FV(F51,H51,,D51)-D51</f>
         <v>1370969.0480099991</v>
       </c>
       <c r="O54" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>